<commit_message>
Setup sandbox for data set testing
Created copies to allow swapping data without changing previous file or
variant name.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly data sample" sheetId="1" r:id="rId1"/>
     <sheet name="Monthly 10 homes" sheetId="2" r:id="rId2"/>
+    <sheet name="Monthly 10 homes 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="24">
   <si>
     <t>Column Labels</t>
   </si>
@@ -1188,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,4 +2281,1101 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45</v>
+      </c>
+      <c r="H2" s="2">
+        <v>46</v>
+      </c>
+      <c r="I2" s="2">
+        <v>47</v>
+      </c>
+      <c r="J2" s="2">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2">
+        <v>49</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>406.27199999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>318.98999999999995</v>
+      </c>
+      <c r="D4" s="6">
+        <v>675.154</v>
+      </c>
+      <c r="E4" s="6">
+        <v>354.26699999999994</v>
+      </c>
+      <c r="F4" s="6">
+        <v>558.93599999999981</v>
+      </c>
+      <c r="G4" s="6">
+        <v>257.74599999999998</v>
+      </c>
+      <c r="H4" s="6">
+        <v>690.98499999999979</v>
+      </c>
+      <c r="I4" s="6">
+        <v>527.72899999999993</v>
+      </c>
+      <c r="J4" s="6">
+        <v>535.67000000000007</v>
+      </c>
+      <c r="K4" s="6">
+        <v>384.78599999999989</v>
+      </c>
+      <c r="L4" s="6">
+        <v>4710.5349999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>391.24900000000014</v>
+      </c>
+      <c r="C5" s="6">
+        <v>271.78699999999992</v>
+      </c>
+      <c r="D5" s="6">
+        <v>610.51000000000022</v>
+      </c>
+      <c r="E5" s="6">
+        <v>331.23499999999996</v>
+      </c>
+      <c r="F5" s="6">
+        <v>409.15500000000009</v>
+      </c>
+      <c r="G5" s="6">
+        <v>355.06799999999998</v>
+      </c>
+      <c r="H5" s="6">
+        <v>692.18099999999981</v>
+      </c>
+      <c r="I5" s="6">
+        <v>432.83100000000007</v>
+      </c>
+      <c r="J5" s="6">
+        <v>506.02500000000003</v>
+      </c>
+      <c r="K5" s="6">
+        <v>396.22999999999996</v>
+      </c>
+      <c r="L5" s="6">
+        <v>4396.2709999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>319.85600000000005</v>
+      </c>
+      <c r="C6" s="6">
+        <v>281.54799999999994</v>
+      </c>
+      <c r="D6" s="6">
+        <v>537.07299999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <v>228.96600000000004</v>
+      </c>
+      <c r="F6" s="6">
+        <v>216.82600000000002</v>
+      </c>
+      <c r="G6" s="6">
+        <v>296.69999999999993</v>
+      </c>
+      <c r="H6" s="6">
+        <v>634.92500000000007</v>
+      </c>
+      <c r="I6" s="6">
+        <v>347.27100000000002</v>
+      </c>
+      <c r="J6" s="6">
+        <v>314.5089999999999</v>
+      </c>
+      <c r="K6" s="6">
+        <v>291.36200000000002</v>
+      </c>
+      <c r="L6" s="6">
+        <v>3469.0360000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>221.238</v>
+      </c>
+      <c r="C7" s="6">
+        <v>326.07299999999992</v>
+      </c>
+      <c r="D7" s="6">
+        <v>547.10800000000006</v>
+      </c>
+      <c r="E7" s="6">
+        <v>229.934</v>
+      </c>
+      <c r="F7" s="6">
+        <v>237.36300000000003</v>
+      </c>
+      <c r="G7" s="6">
+        <v>275.96299999999997</v>
+      </c>
+      <c r="H7" s="6">
+        <v>710.96200000000022</v>
+      </c>
+      <c r="I7" s="6">
+        <v>354.30100000000004</v>
+      </c>
+      <c r="J7" s="6">
+        <v>326.47699999999998</v>
+      </c>
+      <c r="K7" s="6">
+        <v>330.08099999999985</v>
+      </c>
+      <c r="L7" s="6">
+        <v>3559.4999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>247.71300000000002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>400.83600000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>553.18399999999997</v>
+      </c>
+      <c r="E8" s="6">
+        <v>244.37999999999994</v>
+      </c>
+      <c r="F8" s="6">
+        <v>193.68400000000005</v>
+      </c>
+      <c r="G8" s="6">
+        <v>221.959</v>
+      </c>
+      <c r="H8" s="6">
+        <v>660.11999999999978</v>
+      </c>
+      <c r="I8" s="6">
+        <v>397.04199999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <v>274.30599999999993</v>
+      </c>
+      <c r="K8" s="6">
+        <v>377.53799999999995</v>
+      </c>
+      <c r="L8" s="6">
+        <v>3570.7619999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>297.50299999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>365.10000000000008</v>
+      </c>
+      <c r="D9" s="6">
+        <v>653.93000000000006</v>
+      </c>
+      <c r="E9" s="6">
+        <v>341.09199999999998</v>
+      </c>
+      <c r="F9" s="6">
+        <v>339.72799999999995</v>
+      </c>
+      <c r="G9" s="6">
+        <v>236.94299999999998</v>
+      </c>
+      <c r="H9" s="6">
+        <v>695.90700000000004</v>
+      </c>
+      <c r="I9" s="6">
+        <v>387.185</v>
+      </c>
+      <c r="J9" s="6">
+        <v>285.101</v>
+      </c>
+      <c r="K9" s="6">
+        <v>517.99900000000014</v>
+      </c>
+      <c r="L9" s="6">
+        <v>4120.4880000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>325.54700000000003</v>
+      </c>
+      <c r="C10" s="6">
+        <v>348.14399999999995</v>
+      </c>
+      <c r="D10" s="6">
+        <v>633.2969999999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>404.13799999999998</v>
+      </c>
+      <c r="F10" s="6">
+        <v>289.24399999999997</v>
+      </c>
+      <c r="G10" s="6">
+        <v>258.39699999999999</v>
+      </c>
+      <c r="H10" s="6">
+        <v>731.07199999999989</v>
+      </c>
+      <c r="I10" s="6">
+        <v>577.52899999999977</v>
+      </c>
+      <c r="J10" s="6">
+        <v>283.29200000000003</v>
+      </c>
+      <c r="K10" s="6">
+        <v>717.49099999999976</v>
+      </c>
+      <c r="L10" s="6">
+        <v>4568.1509999999989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>240.02799999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>278.899</v>
+      </c>
+      <c r="D11" s="6">
+        <v>543.77600000000007</v>
+      </c>
+      <c r="E11" s="6">
+        <v>241.11599999999996</v>
+      </c>
+      <c r="F11" s="6">
+        <v>277.209</v>
+      </c>
+      <c r="G11" s="6">
+        <v>301.53699999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>646.63799999999992</v>
+      </c>
+      <c r="I11" s="6">
+        <v>448.09800000000007</v>
+      </c>
+      <c r="J11" s="6">
+        <v>226.14300000000006</v>
+      </c>
+      <c r="K11" s="6">
+        <v>385.00799999999998</v>
+      </c>
+      <c r="L11" s="6">
+        <v>3588.4519999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>262.91699999999997</v>
+      </c>
+      <c r="C12" s="6">
+        <v>333.04499999999996</v>
+      </c>
+      <c r="D12" s="6">
+        <v>556.98500000000013</v>
+      </c>
+      <c r="E12" s="6">
+        <v>266.43699999999995</v>
+      </c>
+      <c r="F12" s="6">
+        <v>264.45899999999995</v>
+      </c>
+      <c r="G12" s="6">
+        <v>324.4199999999999</v>
+      </c>
+      <c r="H12" s="6">
+        <v>677.14399999999989</v>
+      </c>
+      <c r="I12" s="6">
+        <v>472.14100000000008</v>
+      </c>
+      <c r="J12" s="6">
+        <v>282.07200000000012</v>
+      </c>
+      <c r="K12" s="6">
+        <v>384.86399999999992</v>
+      </c>
+      <c r="L12" s="6">
+        <v>3824.4839999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>229.59900000000002</v>
+      </c>
+      <c r="C13" s="6">
+        <v>297.57500000000005</v>
+      </c>
+      <c r="D13" s="6">
+        <v>505.92999999999989</v>
+      </c>
+      <c r="E13" s="6">
+        <v>252.50499999999997</v>
+      </c>
+      <c r="F13" s="6">
+        <v>208.80099999999999</v>
+      </c>
+      <c r="G13" s="6">
+        <v>253.31900000000005</v>
+      </c>
+      <c r="H13" s="6">
+        <v>644.601</v>
+      </c>
+      <c r="I13" s="6">
+        <v>391.11500000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>269.27500000000003</v>
+      </c>
+      <c r="K13" s="6">
+        <v>330.11200000000002</v>
+      </c>
+      <c r="L13" s="6">
+        <v>3382.8319999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>152.49299999999999</v>
+      </c>
+      <c r="C14" s="6">
+        <v>294.72900000000004</v>
+      </c>
+      <c r="D14" s="6">
+        <v>534.91200000000015</v>
+      </c>
+      <c r="E14" s="6">
+        <v>252.84699999999998</v>
+      </c>
+      <c r="F14" s="6">
+        <v>581.01700000000005</v>
+      </c>
+      <c r="G14" s="6">
+        <v>288.65700000000004</v>
+      </c>
+      <c r="H14" s="6">
+        <v>667.58799999999997</v>
+      </c>
+      <c r="I14" s="6">
+        <v>421.49</v>
+      </c>
+      <c r="J14" s="6">
+        <v>341.07899999999995</v>
+      </c>
+      <c r="K14" s="6">
+        <v>316.48500000000007</v>
+      </c>
+      <c r="L14" s="6">
+        <v>3851.297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>282.04499999999996</v>
+      </c>
+      <c r="C15" s="6">
+        <v>213.60999999999999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>669.38600000000008</v>
+      </c>
+      <c r="E15" s="6">
+        <v>244.38900000000001</v>
+      </c>
+      <c r="F15" s="6">
+        <v>537.41100000000006</v>
+      </c>
+      <c r="G15" s="6">
+        <v>316.56799999999993</v>
+      </c>
+      <c r="H15" s="6">
+        <v>645.38599999999997</v>
+      </c>
+      <c r="I15" s="6">
+        <v>496.23400000000004</v>
+      </c>
+      <c r="J15" s="6">
+        <v>261.34699999999998</v>
+      </c>
+      <c r="K15" s="6">
+        <v>394.03300000000007</v>
+      </c>
+      <c r="L15" s="6">
+        <v>4060.4090000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3376.46</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3730.3359999999998</v>
+      </c>
+      <c r="D16" s="8">
+        <v>7021.2450000000008</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3391.3059999999996</v>
+      </c>
+      <c r="F16" s="8">
+        <v>4113.8329999999996</v>
+      </c>
+      <c r="G16" s="8">
+        <v>3387.2769999999996</v>
+      </c>
+      <c r="H16" s="8">
+        <v>8097.509</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5252.9660000000003</v>
+      </c>
+      <c r="J16" s="8">
+        <v>3905.2960000000003</v>
+      </c>
+      <c r="K16" s="8">
+        <v>4825.9889999999996</v>
+      </c>
+      <c r="L16" s="8">
+        <v>47102.216999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>64.875</v>
+      </c>
+      <c r="C18" s="6">
+        <v>68.061999999999983</v>
+      </c>
+      <c r="D18" s="6">
+        <v>222.16899999999998</v>
+      </c>
+      <c r="E18" s="6">
+        <v>85.350999999999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>52.38</v>
+      </c>
+      <c r="G18" s="6">
+        <v>63.415999999999983</v>
+      </c>
+      <c r="H18" s="6">
+        <v>106.05799999999999</v>
+      </c>
+      <c r="I18" s="6">
+        <v>80.919999999999987</v>
+      </c>
+      <c r="J18" s="6">
+        <v>109.13099999999997</v>
+      </c>
+      <c r="K18" s="6">
+        <v>91.373999999999995</v>
+      </c>
+      <c r="L18" s="6">
+        <v>943.73599999999988</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6">
+        <v>101.67499999999997</v>
+      </c>
+      <c r="C19" s="6">
+        <v>96.578000000000003</v>
+      </c>
+      <c r="D19" s="6">
+        <v>370.40100000000001</v>
+      </c>
+      <c r="E19" s="6">
+        <v>126.02299999999998</v>
+      </c>
+      <c r="F19" s="6">
+        <v>80.582999999999998</v>
+      </c>
+      <c r="G19" s="6">
+        <v>111.73299999999999</v>
+      </c>
+      <c r="H19" s="6">
+        <v>152.304</v>
+      </c>
+      <c r="I19" s="6">
+        <v>113.61600000000001</v>
+      </c>
+      <c r="J19" s="6">
+        <v>217.82599999999999</v>
+      </c>
+      <c r="K19" s="6">
+        <v>129.13499999999999</v>
+      </c>
+      <c r="L19" s="6">
+        <v>1499.874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6">
+        <v>119.50399999999999</v>
+      </c>
+      <c r="C20" s="6">
+        <v>121.44</v>
+      </c>
+      <c r="D20" s="6">
+        <v>466.81799999999993</v>
+      </c>
+      <c r="E20" s="6">
+        <v>154.94699999999997</v>
+      </c>
+      <c r="F20" s="6">
+        <v>107.56699999999998</v>
+      </c>
+      <c r="G20" s="6">
+        <v>185.50200000000001</v>
+      </c>
+      <c r="H20" s="6">
+        <v>168.24700000000001</v>
+      </c>
+      <c r="I20" s="6">
+        <v>135.96100000000001</v>
+      </c>
+      <c r="J20" s="6">
+        <v>283.38700000000006</v>
+      </c>
+      <c r="K20" s="6">
+        <v>147.71600000000004</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1891.0890000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6">
+        <v>128.70500000000001</v>
+      </c>
+      <c r="C21" s="6">
+        <v>138.22</v>
+      </c>
+      <c r="D21" s="6">
+        <v>506.53899999999999</v>
+      </c>
+      <c r="E21" s="6">
+        <v>188.00899999999999</v>
+      </c>
+      <c r="F21" s="6">
+        <v>129.08799999999999</v>
+      </c>
+      <c r="G21" s="6">
+        <v>249.62000000000003</v>
+      </c>
+      <c r="H21" s="6">
+        <v>179.16300000000004</v>
+      </c>
+      <c r="I21" s="6">
+        <v>153.74500000000003</v>
+      </c>
+      <c r="J21" s="6">
+        <v>326.00900000000001</v>
+      </c>
+      <c r="K21" s="6">
+        <v>152.04999999999995</v>
+      </c>
+      <c r="L21" s="6">
+        <v>2151.1480000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6">
+        <v>103.43</v>
+      </c>
+      <c r="C22" s="6">
+        <v>120.44500000000001</v>
+      </c>
+      <c r="D22" s="6">
+        <v>409.55500000000001</v>
+      </c>
+      <c r="E22" s="6">
+        <v>178.89100000000002</v>
+      </c>
+      <c r="F22" s="6">
+        <v>116.2</v>
+      </c>
+      <c r="G22" s="6">
+        <v>228.75600000000003</v>
+      </c>
+      <c r="H22" s="6">
+        <v>150.25200000000001</v>
+      </c>
+      <c r="I22" s="6">
+        <v>131.77800000000002</v>
+      </c>
+      <c r="J22" s="6">
+        <v>300.93700000000007</v>
+      </c>
+      <c r="K22" s="6">
+        <v>130.52199999999999</v>
+      </c>
+      <c r="L22" s="6">
+        <v>1870.7660000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="6">
+        <v>111.006</v>
+      </c>
+      <c r="C23" s="6">
+        <v>136.43800000000002</v>
+      </c>
+      <c r="D23" s="6">
+        <v>456.90600000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>201.34900000000002</v>
+      </c>
+      <c r="F23" s="6">
+        <v>130.827</v>
+      </c>
+      <c r="G23" s="6">
+        <v>251.40600000000001</v>
+      </c>
+      <c r="H23" s="6">
+        <v>155.68400000000003</v>
+      </c>
+      <c r="I23" s="6">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="J23" s="6">
+        <v>319.82500000000005</v>
+      </c>
+      <c r="K23" s="6">
+        <v>141.303</v>
+      </c>
+      <c r="L23" s="6">
+        <v>2043.8540000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="6">
+        <v>112.99000000000002</v>
+      </c>
+      <c r="C24" s="6">
+        <v>133.142</v>
+      </c>
+      <c r="D24" s="6">
+        <v>432.70800000000003</v>
+      </c>
+      <c r="E24" s="6">
+        <v>188.85600000000002</v>
+      </c>
+      <c r="F24" s="6">
+        <v>129.11399999999998</v>
+      </c>
+      <c r="G24" s="6">
+        <v>245.78100000000006</v>
+      </c>
+      <c r="H24" s="6">
+        <v>156.32499999999999</v>
+      </c>
+      <c r="I24" s="6">
+        <v>141.29899999999998</v>
+      </c>
+      <c r="J24" s="6">
+        <v>313.95600000000007</v>
+      </c>
+      <c r="K24" s="6">
+        <v>137.828</v>
+      </c>
+      <c r="L24" s="6">
+        <v>1991.999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6">
+        <v>98.518000000000015</v>
+      </c>
+      <c r="C25" s="6">
+        <v>114.45700000000002</v>
+      </c>
+      <c r="D25" s="6">
+        <v>411.76100000000002</v>
+      </c>
+      <c r="E25" s="6">
+        <v>157.23799999999997</v>
+      </c>
+      <c r="F25" s="6">
+        <v>105.85400000000001</v>
+      </c>
+      <c r="G25" s="6">
+        <v>199.86899999999997</v>
+      </c>
+      <c r="H25" s="6">
+        <v>137.363</v>
+      </c>
+      <c r="I25" s="6">
+        <v>124.30600000000001</v>
+      </c>
+      <c r="J25" s="6">
+        <v>257.80099999999999</v>
+      </c>
+      <c r="K25" s="6">
+        <v>124.499</v>
+      </c>
+      <c r="L25" s="6">
+        <v>1731.6660000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="6">
+        <v>111.697</v>
+      </c>
+      <c r="C26" s="6">
+        <v>120.01899999999999</v>
+      </c>
+      <c r="D26" s="6">
+        <v>425.90500000000009</v>
+      </c>
+      <c r="E26" s="6">
+        <v>157.94399999999999</v>
+      </c>
+      <c r="F26" s="6">
+        <v>110.45</v>
+      </c>
+      <c r="G26" s="6">
+        <v>202.65599999999998</v>
+      </c>
+      <c r="H26" s="6">
+        <v>153.88999999999999</v>
+      </c>
+      <c r="I26" s="6">
+        <v>133.56999999999996</v>
+      </c>
+      <c r="J26" s="6">
+        <v>279.60700000000003</v>
+      </c>
+      <c r="K26" s="6">
+        <v>135.64100000000002</v>
+      </c>
+      <c r="L26" s="6">
+        <v>1831.3790000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6">
+        <v>91.993999999999986</v>
+      </c>
+      <c r="C27" s="6">
+        <v>90.7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>356.572</v>
+      </c>
+      <c r="E27" s="6">
+        <v>118.15700000000002</v>
+      </c>
+      <c r="F27" s="6">
+        <v>79.431999999999988</v>
+      </c>
+      <c r="G27" s="6">
+        <v>139.21600000000001</v>
+      </c>
+      <c r="H27" s="6">
+        <v>134.75900000000001</v>
+      </c>
+      <c r="I27" s="6">
+        <v>105.11500000000001</v>
+      </c>
+      <c r="J27" s="6">
+        <v>196.13999999999996</v>
+      </c>
+      <c r="K27" s="6">
+        <v>122.11399999999999</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1434.1990000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="6">
+        <v>80.479999999999961</v>
+      </c>
+      <c r="C28" s="6">
+        <v>76.384999999999991</v>
+      </c>
+      <c r="D28" s="6">
+        <v>263.3490000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>98.891999999999982</v>
+      </c>
+      <c r="F28" s="6">
+        <v>61.866000000000014</v>
+      </c>
+      <c r="G28" s="6">
+        <v>115.74799999999998</v>
+      </c>
+      <c r="H28" s="6">
+        <v>114.46799999999999</v>
+      </c>
+      <c r="I28" s="6">
+        <v>90.445999999999984</v>
+      </c>
+      <c r="J28" s="6">
+        <v>146.62799999999999</v>
+      </c>
+      <c r="K28" s="6">
+        <v>103.73099999999999</v>
+      </c>
+      <c r="L28" s="6">
+        <v>1151.9929999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="6">
+        <v>43.441999999999993</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44.253</v>
+      </c>
+      <c r="D29" s="6">
+        <v>155.75900000000001</v>
+      </c>
+      <c r="E29" s="6">
+        <v>61.987999999999985</v>
+      </c>
+      <c r="F29" s="6">
+        <v>33.684999999999995</v>
+      </c>
+      <c r="G29" s="6">
+        <v>66.321999999999989</v>
+      </c>
+      <c r="H29" s="6">
+        <v>69.669000000000011</v>
+      </c>
+      <c r="I29" s="6">
+        <v>57.185999999999986</v>
+      </c>
+      <c r="J29" s="6">
+        <v>75.953000000000003</v>
+      </c>
+      <c r="K29" s="6">
+        <v>60.731999999999985</v>
+      </c>
+      <c r="L29" s="6">
+        <v>668.98900000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1168.316</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1260.1389999999999</v>
+      </c>
+      <c r="D30" s="8">
+        <v>4478.442</v>
+      </c>
+      <c r="E30" s="8">
+        <v>1717.6450000000002</v>
+      </c>
+      <c r="F30" s="8">
+        <v>1137.046</v>
+      </c>
+      <c r="G30" s="8">
+        <v>2060.0250000000001</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1678.1820000000002</v>
+      </c>
+      <c r="I30" s="8">
+        <v>1407.0519999999999</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2827.2000000000003</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1476.645</v>
+      </c>
+      <c r="L30" s="8">
+        <v>19210.692000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add 10 homes for non-solar homes
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="24">
   <si>
     <t>Column Labels</t>
   </si>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,9 +2297,13 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2316,8 +2320,21 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2354,8 +2371,41 @@
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="2">
+        <v>140</v>
+      </c>
+      <c r="O2" s="2">
+        <v>141</v>
+      </c>
+      <c r="P2" s="2">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>143</v>
+      </c>
+      <c r="R2" s="2">
+        <v>144</v>
+      </c>
+      <c r="S2" s="2">
+        <v>145</v>
+      </c>
+      <c r="T2" s="2">
+        <v>146</v>
+      </c>
+      <c r="U2" s="2">
+        <v>147</v>
+      </c>
+      <c r="V2" s="2">
+        <v>148</v>
+      </c>
+      <c r="W2" s="2">
+        <v>149</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2370,8 +2420,19 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2408,8 +2469,41 @@
       <c r="L4" s="6">
         <v>4710.5349999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="6">
+        <v>308.84699999999998</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1200.2460000000001</v>
+      </c>
+      <c r="P4" s="6">
+        <v>427.47500000000002</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>298.30799999999999</v>
+      </c>
+      <c r="R4" s="6">
+        <v>476.20899999999989</v>
+      </c>
+      <c r="S4" s="6">
+        <v>942.68299999999988</v>
+      </c>
+      <c r="T4" s="6">
+        <v>20.208000000000009</v>
+      </c>
+      <c r="U4" s="6">
+        <v>1993.1020000000005</v>
+      </c>
+      <c r="V4" s="6">
+        <v>683.02299999999991</v>
+      </c>
+      <c r="W4" s="6">
+        <v>971.47799999999984</v>
+      </c>
+      <c r="X4" s="6">
+        <v>7321.5790000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2446,8 +2540,41 @@
       <c r="L5" s="6">
         <v>4396.2709999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="6">
+        <v>90.468000000000018</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1242.4160000000002</v>
+      </c>
+      <c r="P5" s="6">
+        <v>333.59700000000004</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>613.74799999999993</v>
+      </c>
+      <c r="R5" s="6">
+        <v>377.04199999999997</v>
+      </c>
+      <c r="S5" s="6">
+        <v>914.59699999999987</v>
+      </c>
+      <c r="T5" s="6">
+        <v>23.495000000000008</v>
+      </c>
+      <c r="U5" s="6">
+        <v>1581.83</v>
+      </c>
+      <c r="V5" s="6">
+        <v>872.21000000000015</v>
+      </c>
+      <c r="W5" s="6">
+        <v>920.82499999999993</v>
+      </c>
+      <c r="X5" s="6">
+        <v>6970.2279999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2484,8 +2611,41 @@
       <c r="L6" s="6">
         <v>3469.0360000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="6">
+        <v>25.860000000000014</v>
+      </c>
+      <c r="O6" s="6">
+        <v>991.01699999999983</v>
+      </c>
+      <c r="P6" s="6">
+        <v>207.721</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>552.56899999999985</v>
+      </c>
+      <c r="R6" s="6">
+        <v>238.55300000000003</v>
+      </c>
+      <c r="S6" s="6">
+        <v>558.07499999999993</v>
+      </c>
+      <c r="T6" s="6">
+        <v>167.68100000000001</v>
+      </c>
+      <c r="U6" s="6">
+        <v>1216.4729999999995</v>
+      </c>
+      <c r="V6" s="6">
+        <v>629.09100000000012</v>
+      </c>
+      <c r="W6" s="6">
+        <v>654.16000000000008</v>
+      </c>
+      <c r="X6" s="6">
+        <v>5241.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -2522,8 +2682,41 @@
       <c r="L7" s="6">
         <v>3559.4999999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="6">
+        <v>100.26500000000006</v>
+      </c>
+      <c r="O7" s="6">
+        <v>961.58100000000013</v>
+      </c>
+      <c r="P7" s="6">
+        <v>332.44299999999998</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>469.18200000000002</v>
+      </c>
+      <c r="R7" s="6">
+        <v>283.30100000000004</v>
+      </c>
+      <c r="S7" s="6">
+        <v>680.51999999999987</v>
+      </c>
+      <c r="T7" s="6">
+        <v>119.196</v>
+      </c>
+      <c r="U7" s="6">
+        <v>884.07700000000023</v>
+      </c>
+      <c r="V7" s="6">
+        <v>435.05400000000009</v>
+      </c>
+      <c r="W7" s="6">
+        <v>665.774</v>
+      </c>
+      <c r="X7" s="6">
+        <v>4931.3930000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -2560,8 +2753,41 @@
       <c r="L8" s="6">
         <v>3570.7619999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="6">
+        <v>139.77800000000002</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1050.5220000000002</v>
+      </c>
+      <c r="P8" s="6">
+        <v>321.64600000000002</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>593.62400000000002</v>
+      </c>
+      <c r="R8" s="6">
+        <v>323.41700000000009</v>
+      </c>
+      <c r="S8" s="6">
+        <v>751.15599999999984</v>
+      </c>
+      <c r="T8" s="6">
+        <v>130.78899999999999</v>
+      </c>
+      <c r="U8" s="6">
+        <v>673.49799999999993</v>
+      </c>
+      <c r="V8" s="6">
+        <v>524.14200000000005</v>
+      </c>
+      <c r="W8" s="6">
+        <v>639.14200000000005</v>
+      </c>
+      <c r="X8" s="6">
+        <v>5147.7139999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -2598,8 +2824,41 @@
       <c r="L9" s="6">
         <v>4120.4880000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="6">
+        <v>56.515999999999991</v>
+      </c>
+      <c r="O9" s="6">
+        <v>1096.4159999999997</v>
+      </c>
+      <c r="P9" s="6">
+        <v>312.05399999999997</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>893.88599999999997</v>
+      </c>
+      <c r="R9" s="6">
+        <v>359.54699999999997</v>
+      </c>
+      <c r="S9" s="6">
+        <v>887.09699999999987</v>
+      </c>
+      <c r="T9" s="6">
+        <v>191.71199999999999</v>
+      </c>
+      <c r="U9" s="6">
+        <v>634.61099999999999</v>
+      </c>
+      <c r="V9" s="6">
+        <v>518.45800000000008</v>
+      </c>
+      <c r="W9" s="6">
+        <v>438.07399999999996</v>
+      </c>
+      <c r="X9" s="6">
+        <v>5388.3710000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -2636,8 +2895,41 @@
       <c r="L10" s="6">
         <v>4568.1509999999989</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="6">
+        <v>72.271000000000001</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1307.8350000000005</v>
+      </c>
+      <c r="P10" s="6">
+        <v>312.95499999999998</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>970.69800000000009</v>
+      </c>
+      <c r="R10" s="6">
+        <v>404.08600000000007</v>
+      </c>
+      <c r="S10" s="6">
+        <v>948.39499999999998</v>
+      </c>
+      <c r="T10" s="6">
+        <v>239.86299999999997</v>
+      </c>
+      <c r="U10" s="6">
+        <v>711.62400000000014</v>
+      </c>
+      <c r="V10" s="6">
+        <v>557.95799999999986</v>
+      </c>
+      <c r="W10" s="6">
+        <v>509.22199999999987</v>
+      </c>
+      <c r="X10" s="6">
+        <v>6034.9070000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2674,8 +2966,41 @@
       <c r="L11" s="6">
         <v>3588.4519999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" s="6">
+        <v>133.57500000000002</v>
+      </c>
+      <c r="O11" s="6">
+        <v>895.93299999999977</v>
+      </c>
+      <c r="P11" s="6">
+        <v>305.38900000000007</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>486.78599999999994</v>
+      </c>
+      <c r="R11" s="6">
+        <v>328.66299999999995</v>
+      </c>
+      <c r="S11" s="6">
+        <v>722.3280000000002</v>
+      </c>
+      <c r="T11" s="6">
+        <v>152.81</v>
+      </c>
+      <c r="U11" s="6">
+        <v>639.41499999999996</v>
+      </c>
+      <c r="V11" s="6">
+        <v>376.78399999999999</v>
+      </c>
+      <c r="W11" s="6">
+        <v>580.29000000000008</v>
+      </c>
+      <c r="X11" s="6">
+        <v>4621.973</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -2712,8 +3037,41 @@
       <c r="L12" s="6">
         <v>3824.4839999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" s="6">
+        <v>145.214</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1028.7910000000002</v>
+      </c>
+      <c r="P12" s="6">
+        <v>337.08999999999992</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>584.53300000000013</v>
+      </c>
+      <c r="R12" s="6">
+        <v>338.99300000000005</v>
+      </c>
+      <c r="S12" s="6">
+        <v>747.72100000000012</v>
+      </c>
+      <c r="T12" s="6">
+        <v>150.125</v>
+      </c>
+      <c r="U12" s="6">
+        <v>725.81299999999987</v>
+      </c>
+      <c r="V12" s="6">
+        <v>419.36500000000007</v>
+      </c>
+      <c r="W12" s="6">
+        <v>625.11400000000003</v>
+      </c>
+      <c r="X12" s="6">
+        <v>5102.759</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -2750,8 +3108,41 @@
       <c r="L13" s="6">
         <v>3382.8319999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" s="6">
+        <v>139.90600000000001</v>
+      </c>
+      <c r="O13" s="6">
+        <v>888.79199999999992</v>
+      </c>
+      <c r="P13" s="6">
+        <v>360.97100000000006</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>450.82300000000004</v>
+      </c>
+      <c r="R13" s="6">
+        <v>299.09100000000001</v>
+      </c>
+      <c r="S13" s="6">
+        <v>627.005</v>
+      </c>
+      <c r="T13" s="6">
+        <v>136.191</v>
+      </c>
+      <c r="U13" s="6">
+        <v>632.56799999999998</v>
+      </c>
+      <c r="V13" s="6">
+        <v>522.92000000000007</v>
+      </c>
+      <c r="W13" s="6">
+        <v>601.59699999999998</v>
+      </c>
+      <c r="X13" s="6">
+        <v>4659.8639999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -2788,8 +3179,41 @@
       <c r="L14" s="6">
         <v>3851.297</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14" s="6">
+        <v>171.21699999999998</v>
+      </c>
+      <c r="O14" s="6">
+        <v>989.17599999999993</v>
+      </c>
+      <c r="P14" s="6">
+        <v>373.00800000000004</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>415.40100000000001</v>
+      </c>
+      <c r="R14" s="6">
+        <v>311.30799999999994</v>
+      </c>
+      <c r="S14" s="6">
+        <v>649.79500000000007</v>
+      </c>
+      <c r="T14" s="6">
+        <v>141.06000000000003</v>
+      </c>
+      <c r="U14" s="6">
+        <v>710.44699999999978</v>
+      </c>
+      <c r="V14" s="6">
+        <v>683.47599999999989</v>
+      </c>
+      <c r="W14" s="6">
+        <v>647.51700000000017</v>
+      </c>
+      <c r="X14" s="6">
+        <v>5092.4049999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -2826,8 +3250,41 @@
       <c r="L15" s="6">
         <v>4060.4090000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15" s="6">
+        <v>263.52500000000003</v>
+      </c>
+      <c r="O15" s="6">
+        <v>887.87300000000005</v>
+      </c>
+      <c r="P15" s="6">
+        <v>461.42199999999985</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>506.76699999999988</v>
+      </c>
+      <c r="R15" s="6">
+        <v>368.11300000000011</v>
+      </c>
+      <c r="S15" s="6">
+        <v>253.16900000000001</v>
+      </c>
+      <c r="T15" s="6">
+        <v>209.05300000000005</v>
+      </c>
+      <c r="U15" s="6">
+        <v>862.51199999999994</v>
+      </c>
+      <c r="V15" s="6">
+        <v>993.9079999999999</v>
+      </c>
+      <c r="W15" s="6">
+        <v>937.83300000000008</v>
+      </c>
+      <c r="X15" s="6">
+        <v>5744.1750000000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -2863,6 +3320,39 @@
       </c>
       <c r="L16" s="8">
         <v>47102.216999999997</v>
+      </c>
+      <c r="N16" s="8">
+        <v>1647.442</v>
+      </c>
+      <c r="O16" s="8">
+        <v>12540.598</v>
+      </c>
+      <c r="P16" s="8">
+        <v>4085.7710000000002</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>6836.3249999999998</v>
+      </c>
+      <c r="R16" s="8">
+        <v>4108.3230000000003</v>
+      </c>
+      <c r="S16" s="8">
+        <v>8682.5409999999993</v>
+      </c>
+      <c r="T16" s="8">
+        <v>1682.183</v>
+      </c>
+      <c r="U16" s="8">
+        <v>11265.970000000001</v>
+      </c>
+      <c r="V16" s="8">
+        <v>7216.3889999999992</v>
+      </c>
+      <c r="W16" s="8">
+        <v>8191.0259999999998</v>
+      </c>
+      <c r="X16" s="8">
+        <v>66256.567999999999</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Switch from 140-149 to 70-79
Non-solar profile changes from 140-149 to 70-79 to avoid "no calculation
result" error.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -2288,7 +2288,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,34 +2372,34 @@
         <v>1</v>
       </c>
       <c r="N2" s="2">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="O2" s="2">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="P2" s="2">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="2">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="R2" s="2">
-        <v>144</v>
+        <v>74</v>
       </c>
       <c r="S2" s="2">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="T2" s="2">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="U2" s="2">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="V2" s="2">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="W2" s="2">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>1</v>
@@ -2470,37 +2470,37 @@
         <v>4710.5349999999999</v>
       </c>
       <c r="N4" s="6">
-        <v>308.84699999999998</v>
+        <v>750.30500000000006</v>
       </c>
       <c r="O4" s="6">
-        <v>1200.2460000000001</v>
+        <v>475.37900000000002</v>
       </c>
       <c r="P4" s="6">
-        <v>427.47500000000002</v>
+        <v>865.04600000000005</v>
       </c>
       <c r="Q4" s="6">
-        <v>298.30799999999999</v>
+        <v>349.54500000000002</v>
       </c>
       <c r="R4" s="6">
-        <v>476.20899999999989</v>
+        <v>612.52699999999993</v>
       </c>
       <c r="S4" s="6">
-        <v>942.68299999999988</v>
+        <v>763.84799999999996</v>
       </c>
       <c r="T4" s="6">
-        <v>20.208000000000009</v>
+        <v>632.32500000000005</v>
       </c>
       <c r="U4" s="6">
-        <v>1993.1020000000005</v>
+        <v>544.19600000000003</v>
       </c>
       <c r="V4" s="6">
-        <v>683.02299999999991</v>
+        <v>540.55799999999999</v>
       </c>
       <c r="W4" s="6">
-        <v>971.47799999999984</v>
+        <v>1035.6550000000002</v>
       </c>
       <c r="X4" s="6">
-        <v>7321.5790000000006</v>
+        <v>6569.384</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -2541,37 +2541,37 @@
         <v>4396.2709999999997</v>
       </c>
       <c r="N5" s="6">
-        <v>90.468000000000018</v>
+        <v>675.21800000000007</v>
       </c>
       <c r="O5" s="6">
-        <v>1242.4160000000002</v>
+        <v>403.73399999999998</v>
       </c>
       <c r="P5" s="6">
-        <v>333.59700000000004</v>
+        <v>663.072</v>
       </c>
       <c r="Q5" s="6">
-        <v>613.74799999999993</v>
+        <v>333.91</v>
       </c>
       <c r="R5" s="6">
-        <v>377.04199999999997</v>
+        <v>512.00699999999995</v>
       </c>
       <c r="S5" s="6">
-        <v>914.59699999999987</v>
+        <v>754.32699999999977</v>
       </c>
       <c r="T5" s="6">
-        <v>23.495000000000008</v>
+        <v>611.33299999999997</v>
       </c>
       <c r="U5" s="6">
-        <v>1581.83</v>
+        <v>517.75</v>
       </c>
       <c r="V5" s="6">
-        <v>872.21000000000015</v>
+        <v>489.7750000000002</v>
       </c>
       <c r="W5" s="6">
-        <v>920.82499999999993</v>
+        <v>833.79700000000014</v>
       </c>
       <c r="X5" s="6">
-        <v>6970.2279999999992</v>
+        <v>5794.9230000000007</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -2612,37 +2612,37 @@
         <v>3469.0360000000005</v>
       </c>
       <c r="N6" s="6">
-        <v>25.860000000000014</v>
+        <v>577.39599999999996</v>
       </c>
       <c r="O6" s="6">
-        <v>991.01699999999983</v>
+        <v>340.2709999999999</v>
       </c>
       <c r="P6" s="6">
-        <v>207.721</v>
+        <v>589.54100000000005</v>
       </c>
       <c r="Q6" s="6">
-        <v>552.56899999999985</v>
+        <v>283.036</v>
       </c>
       <c r="R6" s="6">
-        <v>238.55300000000003</v>
+        <v>505.548</v>
       </c>
       <c r="S6" s="6">
-        <v>558.07499999999993</v>
+        <v>618.42800000000011</v>
       </c>
       <c r="T6" s="6">
-        <v>167.68100000000001</v>
+        <v>408.90699999999998</v>
       </c>
       <c r="U6" s="6">
-        <v>1216.4729999999995</v>
+        <v>325.94499999999999</v>
       </c>
       <c r="V6" s="6">
-        <v>629.09100000000012</v>
+        <v>366.62</v>
       </c>
       <c r="W6" s="6">
-        <v>654.16000000000008</v>
+        <v>518.25200000000007</v>
       </c>
       <c r="X6" s="6">
-        <v>5241.2</v>
+        <v>4533.9440000000004</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -2683,37 +2683,37 @@
         <v>3559.4999999999995</v>
       </c>
       <c r="N7" s="6">
-        <v>100.26500000000006</v>
+        <v>617.60899999999981</v>
       </c>
       <c r="O7" s="6">
-        <v>961.58100000000013</v>
+        <v>305.53399999999993</v>
       </c>
       <c r="P7" s="6">
-        <v>332.44299999999998</v>
+        <v>226.75199999999995</v>
       </c>
       <c r="Q7" s="6">
-        <v>469.18200000000002</v>
+        <v>292.87099999999992</v>
       </c>
       <c r="R7" s="6">
-        <v>283.30100000000004</v>
+        <v>492.17700000000002</v>
       </c>
       <c r="S7" s="6">
-        <v>680.51999999999987</v>
+        <v>893.96800000000007</v>
       </c>
       <c r="T7" s="6">
-        <v>119.196</v>
+        <v>328.92599999999987</v>
       </c>
       <c r="U7" s="6">
-        <v>884.07700000000023</v>
+        <v>297.53299999999996</v>
       </c>
       <c r="V7" s="6">
-        <v>435.05400000000009</v>
+        <v>373.91499999999996</v>
       </c>
       <c r="W7" s="6">
-        <v>665.774</v>
+        <v>362.27799999999985</v>
       </c>
       <c r="X7" s="6">
-        <v>4931.3930000000009</v>
+        <v>4191.5630000000001</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -2754,37 +2754,37 @@
         <v>3570.7619999999997</v>
       </c>
       <c r="N8" s="6">
-        <v>139.77800000000002</v>
+        <v>585.57899999999995</v>
       </c>
       <c r="O8" s="6">
-        <v>1050.5220000000002</v>
+        <v>308.80800000000005</v>
       </c>
       <c r="P8" s="6">
-        <v>321.64600000000002</v>
+        <v>202.89299999999997</v>
       </c>
       <c r="Q8" s="6">
-        <v>593.62400000000002</v>
+        <v>290.65099999999995</v>
       </c>
       <c r="R8" s="6">
-        <v>323.41700000000009</v>
+        <v>433.45099999999991</v>
       </c>
       <c r="S8" s="6">
-        <v>751.15599999999984</v>
+        <v>941.26700000000017</v>
       </c>
       <c r="T8" s="6">
-        <v>130.78899999999999</v>
+        <v>331.72600000000006</v>
       </c>
       <c r="U8" s="6">
-        <v>673.49799999999993</v>
+        <v>145.02599999999998</v>
       </c>
       <c r="V8" s="6">
-        <v>524.14200000000005</v>
+        <v>446.07800000000003</v>
       </c>
       <c r="W8" s="6">
-        <v>639.14200000000005</v>
+        <v>403.32800000000003</v>
       </c>
       <c r="X8" s="6">
-        <v>5147.7139999999999</v>
+        <v>4088.8070000000002</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -2825,37 +2825,37 @@
         <v>4120.4880000000003</v>
       </c>
       <c r="N9" s="6">
-        <v>56.515999999999991</v>
+        <v>706.90499999999986</v>
       </c>
       <c r="O9" s="6">
-        <v>1096.4159999999997</v>
+        <v>326.69699999999995</v>
       </c>
       <c r="P9" s="6">
-        <v>312.05399999999997</v>
+        <v>179.80199999999999</v>
       </c>
       <c r="Q9" s="6">
-        <v>893.88599999999997</v>
+        <v>306.29199999999997</v>
       </c>
       <c r="R9" s="6">
-        <v>359.54699999999997</v>
+        <v>408.25999999999993</v>
       </c>
       <c r="S9" s="6">
-        <v>887.09699999999987</v>
+        <v>1047.1130000000003</v>
       </c>
       <c r="T9" s="6">
-        <v>191.71199999999999</v>
+        <v>337.71999999999986</v>
       </c>
       <c r="U9" s="6">
-        <v>634.61099999999999</v>
+        <v>154.22899999999998</v>
       </c>
       <c r="V9" s="6">
-        <v>518.45800000000008</v>
+        <v>513.89399999999989</v>
       </c>
       <c r="W9" s="6">
-        <v>438.07399999999996</v>
+        <v>472.02699999999999</v>
       </c>
       <c r="X9" s="6">
-        <v>5388.3710000000001</v>
+        <v>4452.9389999999994</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -2896,37 +2896,37 @@
         <v>4568.1509999999989</v>
       </c>
       <c r="N10" s="6">
-        <v>72.271000000000001</v>
+        <v>757.46800000000007</v>
       </c>
       <c r="O10" s="6">
-        <v>1307.8350000000005</v>
+        <v>410.41600000000011</v>
       </c>
       <c r="P10" s="6">
-        <v>312.95499999999998</v>
+        <v>188.42</v>
       </c>
       <c r="Q10" s="6">
-        <v>970.69800000000009</v>
+        <v>387.02399999999994</v>
       </c>
       <c r="R10" s="6">
-        <v>404.08600000000007</v>
+        <v>331.834</v>
       </c>
       <c r="S10" s="6">
-        <v>948.39499999999998</v>
+        <v>794.53099999999995</v>
       </c>
       <c r="T10" s="6">
-        <v>239.86299999999997</v>
+        <v>365.262</v>
       </c>
       <c r="U10" s="6">
-        <v>711.62400000000014</v>
+        <v>212.88</v>
       </c>
       <c r="V10" s="6">
-        <v>557.95799999999986</v>
+        <v>530.54</v>
       </c>
       <c r="W10" s="6">
-        <v>509.22199999999987</v>
+        <v>556.7320000000002</v>
       </c>
       <c r="X10" s="6">
-        <v>6034.9070000000002</v>
+        <v>4535.1070000000009</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -2967,37 +2967,37 @@
         <v>3588.4519999999998</v>
       </c>
       <c r="N11" s="6">
-        <v>133.57500000000002</v>
+        <v>561.92199999999991</v>
       </c>
       <c r="O11" s="6">
-        <v>895.93299999999977</v>
+        <v>377.6160000000001</v>
       </c>
       <c r="P11" s="6">
-        <v>305.38900000000007</v>
+        <v>180.827</v>
       </c>
       <c r="Q11" s="6">
-        <v>486.78599999999994</v>
+        <v>280.07100000000008</v>
       </c>
       <c r="R11" s="6">
-        <v>328.66299999999995</v>
+        <v>340.65400000000005</v>
       </c>
       <c r="S11" s="6">
-        <v>722.3280000000002</v>
+        <v>886.77499999999986</v>
       </c>
       <c r="T11" s="6">
-        <v>152.81</v>
+        <v>289.52900000000005</v>
       </c>
       <c r="U11" s="6">
-        <v>639.41499999999996</v>
+        <v>259.5150000000001</v>
       </c>
       <c r="V11" s="6">
-        <v>376.78399999999999</v>
+        <v>369.423</v>
       </c>
       <c r="W11" s="6">
-        <v>580.29000000000008</v>
+        <v>314.25399999999996</v>
       </c>
       <c r="X11" s="6">
-        <v>4621.973</v>
+        <v>3860.5859999999993</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -3038,37 +3038,37 @@
         <v>3824.4839999999999</v>
       </c>
       <c r="N12" s="6">
-        <v>145.214</v>
+        <v>675.10800000000006</v>
       </c>
       <c r="O12" s="6">
-        <v>1028.7910000000002</v>
+        <v>416.53399999999993</v>
       </c>
       <c r="P12" s="6">
-        <v>337.08999999999992</v>
+        <v>200.37800000000007</v>
       </c>
       <c r="Q12" s="6">
-        <v>584.53300000000013</v>
+        <v>292.74699999999996</v>
       </c>
       <c r="R12" s="6">
-        <v>338.99300000000005</v>
+        <v>354.21100000000013</v>
       </c>
       <c r="S12" s="6">
-        <v>747.72100000000012</v>
+        <v>986.81800000000032</v>
       </c>
       <c r="T12" s="6">
-        <v>150.125</v>
+        <v>324.43299999999999</v>
       </c>
       <c r="U12" s="6">
-        <v>725.81299999999987</v>
+        <v>293.423</v>
       </c>
       <c r="V12" s="6">
-        <v>419.36500000000007</v>
+        <v>492.92199999999991</v>
       </c>
       <c r="W12" s="6">
-        <v>625.11400000000003</v>
+        <v>393.30499999999989</v>
       </c>
       <c r="X12" s="6">
-        <v>5102.759</v>
+        <v>4429.8790000000008</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -3109,37 +3109,37 @@
         <v>3382.8319999999999</v>
       </c>
       <c r="N13" s="6">
-        <v>139.90600000000001</v>
+        <v>520.13099999999997</v>
       </c>
       <c r="O13" s="6">
-        <v>888.79199999999992</v>
+        <v>470.43400000000003</v>
       </c>
       <c r="P13" s="6">
-        <v>360.97100000000006</v>
+        <v>237.86199999999999</v>
       </c>
       <c r="Q13" s="6">
-        <v>450.82300000000004</v>
+        <v>318.95699999999999</v>
       </c>
       <c r="R13" s="6">
-        <v>299.09100000000001</v>
+        <v>412.42900000000003</v>
       </c>
       <c r="S13" s="6">
-        <v>627.005</v>
+        <v>656.51600000000019</v>
       </c>
       <c r="T13" s="6">
-        <v>136.191</v>
+        <v>360.36699999999996</v>
       </c>
       <c r="U13" s="6">
-        <v>632.56799999999998</v>
+        <v>205.851</v>
       </c>
       <c r="V13" s="6">
-        <v>522.92000000000007</v>
+        <v>480.70799999999997</v>
       </c>
       <c r="W13" s="6">
-        <v>601.59699999999998</v>
+        <v>344.57099999999991</v>
       </c>
       <c r="X13" s="6">
-        <v>4659.8639999999996</v>
+        <v>4007.826</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -3180,37 +3180,37 @@
         <v>3851.297</v>
       </c>
       <c r="N14" s="6">
-        <v>171.21699999999998</v>
+        <v>613.77</v>
       </c>
       <c r="O14" s="6">
-        <v>989.17599999999993</v>
+        <v>480.87599999999998</v>
       </c>
       <c r="P14" s="6">
-        <v>373.00800000000004</v>
+        <v>612.755</v>
       </c>
       <c r="Q14" s="6">
-        <v>415.40100000000001</v>
+        <v>322.15600000000001</v>
       </c>
       <c r="R14" s="6">
-        <v>311.30799999999994</v>
+        <v>575.75500000000011</v>
       </c>
       <c r="S14" s="6">
-        <v>649.79500000000007</v>
+        <v>635.25099999999975</v>
       </c>
       <c r="T14" s="6">
-        <v>141.06000000000003</v>
+        <v>516.07800000000009</v>
       </c>
       <c r="U14" s="6">
-        <v>710.44699999999978</v>
+        <v>282.916</v>
       </c>
       <c r="V14" s="6">
-        <v>683.47599999999989</v>
+        <v>572.75</v>
       </c>
       <c r="W14" s="6">
-        <v>647.51700000000017</v>
+        <v>554.29399999999976</v>
       </c>
       <c r="X14" s="6">
-        <v>5092.4049999999997</v>
+        <v>5166.6009999999997</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -3251,37 +3251,37 @@
         <v>4060.4090000000001</v>
       </c>
       <c r="N15" s="6">
-        <v>263.52500000000003</v>
+        <v>721.53199999999993</v>
       </c>
       <c r="O15" s="6">
-        <v>887.87300000000005</v>
+        <v>511.83499999999992</v>
       </c>
       <c r="P15" s="6">
-        <v>461.42199999999985</v>
+        <v>703.19900000000007</v>
       </c>
       <c r="Q15" s="6">
-        <v>506.76699999999988</v>
+        <v>364.64300000000003</v>
       </c>
       <c r="R15" s="6">
-        <v>368.11300000000011</v>
+        <v>794.42600000000004</v>
       </c>
       <c r="S15" s="6">
-        <v>253.16900000000001</v>
+        <v>622.15300000000002</v>
       </c>
       <c r="T15" s="6">
-        <v>209.05300000000005</v>
+        <v>598.69900000000007</v>
       </c>
       <c r="U15" s="6">
-        <v>862.51199999999994</v>
+        <v>428.50799999999992</v>
       </c>
       <c r="V15" s="6">
-        <v>993.9079999999999</v>
+        <v>586.85</v>
       </c>
       <c r="W15" s="6">
-        <v>937.83300000000008</v>
+        <v>690.64300000000026</v>
       </c>
       <c r="X15" s="6">
-        <v>5744.1750000000011</v>
+        <v>6022.4879999999994</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -3322,37 +3322,37 @@
         <v>47102.216999999997</v>
       </c>
       <c r="N16" s="8">
-        <v>1647.442</v>
+        <v>7762.9430000000002</v>
       </c>
       <c r="O16" s="8">
-        <v>12540.598</v>
+        <v>4828.134</v>
       </c>
       <c r="P16" s="8">
-        <v>4085.7710000000002</v>
+        <v>4850.5470000000005</v>
       </c>
       <c r="Q16" s="8">
-        <v>6836.3249999999998</v>
+        <v>3821.9029999999993</v>
       </c>
       <c r="R16" s="8">
-        <v>4108.3230000000003</v>
+        <v>5773.2790000000005</v>
       </c>
       <c r="S16" s="8">
-        <v>8682.5409999999993</v>
+        <v>9600.9950000000008</v>
       </c>
       <c r="T16" s="8">
-        <v>1682.183</v>
+        <v>5105.3050000000003</v>
       </c>
       <c r="U16" s="8">
-        <v>11265.970000000001</v>
+        <v>3667.7719999999995</v>
       </c>
       <c r="V16" s="8">
-        <v>7216.3889999999992</v>
+        <v>5764.0329999999994</v>
       </c>
       <c r="W16" s="8">
-        <v>8191.0259999999998</v>
+        <v>6479.1360000000004</v>
       </c>
       <c r="X16" s="8">
-        <v>66256.567999999999</v>
+        <v>57654.046999999999</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Re-enable non solar homes
Also add additional tables on calculation table.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -10,8 +10,9 @@
     <sheet name="Monthly data sample" sheetId="1" r:id="rId1"/>
     <sheet name="Monthly 10 homes" sheetId="2" r:id="rId2"/>
     <sheet name="Monthly 10 homes 2" sheetId="3" r:id="rId3"/>
+    <sheet name="40-49 extra calc" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,8 +21,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="N3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the energy left after using up all generations. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This one indicates the energy import variance between homes. Specifically, one home and the home next right to it. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This one is actual power flow between two homes. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="28">
   <si>
     <t>Column Labels</t>
   </si>
@@ -94,12 +177,24 @@
   <si>
     <t>Row Labels</t>
   </si>
+  <si>
+    <t>GC-GG</t>
+  </si>
+  <si>
+    <t>MG1-MG2</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>delta MG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +209,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -178,12 +286,82 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -200,7 +378,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="400080"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1190,7 +1368,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L16"/>
+      <selection activeCell="L30" sqref="A1:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,7 +2466,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,4 +4046,2208 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U14" sqref="U14:U23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9" customWidth="1"/>
+    <col min="14" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45</v>
+      </c>
+      <c r="H2" s="2">
+        <v>46</v>
+      </c>
+      <c r="I2" s="2">
+        <v>47</v>
+      </c>
+      <c r="J2" s="2">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2">
+        <v>49</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>406.27199999999999</v>
+      </c>
+      <c r="C4" s="6">
+        <v>318.98999999999995</v>
+      </c>
+      <c r="D4" s="6">
+        <v>675.154</v>
+      </c>
+      <c r="E4" s="6">
+        <v>354.26699999999994</v>
+      </c>
+      <c r="F4" s="6">
+        <v>558.93599999999981</v>
+      </c>
+      <c r="G4" s="6">
+        <v>257.74599999999998</v>
+      </c>
+      <c r="H4" s="6">
+        <v>690.98499999999979</v>
+      </c>
+      <c r="I4" s="6">
+        <v>527.72899999999993</v>
+      </c>
+      <c r="J4" s="6">
+        <v>535.67000000000007</v>
+      </c>
+      <c r="K4" s="6">
+        <v>384.78599999999989</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4">
+        <f>B4-B18</f>
+        <v>341.39699999999999</v>
+      </c>
+      <c r="O4">
+        <f>O32-O33</f>
+        <v>14.409162807595976</v>
+      </c>
+      <c r="P4">
+        <v>14.3471230819257</v>
+      </c>
+      <c r="Q4">
+        <v>359.382062970292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>391.24900000000014</v>
+      </c>
+      <c r="C5" s="6">
+        <v>271.78699999999992</v>
+      </c>
+      <c r="D5" s="6">
+        <v>610.51000000000022</v>
+      </c>
+      <c r="E5" s="6">
+        <v>331.23499999999996</v>
+      </c>
+      <c r="F5" s="6">
+        <v>409.15500000000009</v>
+      </c>
+      <c r="G5" s="6">
+        <v>355.06799999999998</v>
+      </c>
+      <c r="H5" s="6">
+        <v>692.18099999999981</v>
+      </c>
+      <c r="I5" s="6">
+        <v>432.83100000000007</v>
+      </c>
+      <c r="J5" s="6">
+        <v>506.02500000000003</v>
+      </c>
+      <c r="K5" s="6">
+        <v>396.22999999999996</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5">
+        <f>C4-C18</f>
+        <v>250.92799999999997</v>
+      </c>
+      <c r="O5">
+        <f>O33-O34</f>
+        <v>27.527159996833007</v>
+      </c>
+      <c r="P5">
+        <v>104.84722502375099</v>
+      </c>
+      <c r="Q5">
+        <v>344.97290016269602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>319.85600000000005</v>
+      </c>
+      <c r="C6" s="6">
+        <v>281.54799999999994</v>
+      </c>
+      <c r="D6" s="6">
+        <v>537.07299999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <v>228.96600000000004</v>
+      </c>
+      <c r="F6" s="6">
+        <v>216.82600000000002</v>
+      </c>
+      <c r="G6" s="6">
+        <v>296.69999999999993</v>
+      </c>
+      <c r="H6" s="6">
+        <v>634.92500000000007</v>
+      </c>
+      <c r="I6" s="6">
+        <v>347.27100000000002</v>
+      </c>
+      <c r="J6" s="6">
+        <v>314.5089999999999</v>
+      </c>
+      <c r="K6" s="6">
+        <v>291.36200000000002</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6">
+        <f>D4-D18</f>
+        <v>452.98500000000001</v>
+      </c>
+      <c r="O6">
+        <f>O34-O35</f>
+        <v>-12.334556302633985</v>
+      </c>
+      <c r="P6">
+        <v>-34.209786416514099</v>
+      </c>
+      <c r="Q6">
+        <v>317.44574016586301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>221.238</v>
+      </c>
+      <c r="C7" s="6">
+        <v>326.07299999999992</v>
+      </c>
+      <c r="D7" s="6">
+        <v>547.10800000000006</v>
+      </c>
+      <c r="E7" s="6">
+        <v>229.934</v>
+      </c>
+      <c r="F7" s="6">
+        <v>237.36300000000003</v>
+      </c>
+      <c r="G7" s="6">
+        <v>275.96299999999997</v>
+      </c>
+      <c r="H7" s="6">
+        <v>710.96200000000022</v>
+      </c>
+      <c r="I7" s="6">
+        <v>354.30100000000004</v>
+      </c>
+      <c r="J7" s="6">
+        <v>326.47699999999998</v>
+      </c>
+      <c r="K7" s="6">
+        <v>330.08099999999985</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7">
+        <f>E4-E18</f>
+        <v>268.91599999999994</v>
+      </c>
+      <c r="O7">
+        <f>O35-O36</f>
+        <v>-144.894823774457</v>
+      </c>
+      <c r="P7">
+        <v>23.046098585389</v>
+      </c>
+      <c r="Q7">
+        <v>329.780296468497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>247.71300000000002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>400.83600000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>553.18399999999997</v>
+      </c>
+      <c r="E8" s="6">
+        <v>244.37999999999994</v>
+      </c>
+      <c r="F8" s="6">
+        <v>193.68400000000005</v>
+      </c>
+      <c r="G8" s="6">
+        <v>221.959</v>
+      </c>
+      <c r="H8" s="6">
+        <v>660.11999999999978</v>
+      </c>
+      <c r="I8" s="6">
+        <v>397.04199999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <v>274.30599999999993</v>
+      </c>
+      <c r="K8" s="6">
+        <v>377.53799999999995</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8">
+        <f>F4-F18</f>
+        <v>506.55599999999981</v>
+      </c>
+      <c r="O8">
+        <f>O36-O37</f>
+        <v>108.56715726058798</v>
+      </c>
+      <c r="P8">
+        <v>-15.604841171438499</v>
+      </c>
+      <c r="Q8">
+        <v>474.67512024295399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>297.50299999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>365.10000000000008</v>
+      </c>
+      <c r="D9" s="6">
+        <v>653.93000000000006</v>
+      </c>
+      <c r="E9" s="6">
+        <v>341.09199999999998</v>
+      </c>
+      <c r="F9" s="6">
+        <v>339.72799999999995</v>
+      </c>
+      <c r="G9" s="6">
+        <v>236.94299999999998</v>
+      </c>
+      <c r="H9" s="6">
+        <v>695.90700000000004</v>
+      </c>
+      <c r="I9" s="6">
+        <v>387.185</v>
+      </c>
+      <c r="J9" s="6">
+        <v>285.101</v>
+      </c>
+      <c r="K9" s="6">
+        <v>517.99900000000014</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9">
+        <f>G4-G18</f>
+        <v>194.32999999999998</v>
+      </c>
+      <c r="O9">
+        <f>O37-O38</f>
+        <v>-106.228484161067</v>
+      </c>
+      <c r="P9">
+        <v>151.735678549287</v>
+      </c>
+      <c r="Q9">
+        <v>366.10796298236602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>325.54700000000003</v>
+      </c>
+      <c r="C10" s="6">
+        <v>348.14399999999995</v>
+      </c>
+      <c r="D10" s="6">
+        <v>633.2969999999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>404.13799999999998</v>
+      </c>
+      <c r="F10" s="6">
+        <v>289.24399999999997</v>
+      </c>
+      <c r="G10" s="6">
+        <v>258.39699999999999</v>
+      </c>
+      <c r="H10" s="6">
+        <v>731.07199999999989</v>
+      </c>
+      <c r="I10" s="6">
+        <v>577.52899999999977</v>
+      </c>
+      <c r="J10" s="6">
+        <v>283.29200000000003</v>
+      </c>
+      <c r="K10" s="6">
+        <v>717.49099999999976</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10">
+        <f>H4-H18</f>
+        <v>584.92699999999979</v>
+      </c>
+      <c r="O10">
+        <f>O38-O39</f>
+        <v>154.86155125419504</v>
+      </c>
+      <c r="P10">
+        <v>21.453096342636801</v>
+      </c>
+      <c r="Q10">
+        <v>472.33644714343302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>240.02799999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>278.899</v>
+      </c>
+      <c r="D11" s="6">
+        <v>543.77600000000007</v>
+      </c>
+      <c r="E11" s="6">
+        <v>241.11599999999996</v>
+      </c>
+      <c r="F11" s="6">
+        <v>277.209</v>
+      </c>
+      <c r="G11" s="6">
+        <v>301.53699999999998</v>
+      </c>
+      <c r="H11" s="6">
+        <v>646.63799999999992</v>
+      </c>
+      <c r="I11" s="6">
+        <v>448.09800000000007</v>
+      </c>
+      <c r="J11" s="6">
+        <v>226.14300000000006</v>
+      </c>
+      <c r="K11" s="6">
+        <v>385.00799999999998</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11">
+        <f>I4-I18</f>
+        <v>446.80899999999997</v>
+      </c>
+      <c r="O11">
+        <f>O39-O40</f>
+        <v>-154.05122364076601</v>
+      </c>
+      <c r="P11">
+        <v>-112.45443697595201</v>
+      </c>
+      <c r="Q11">
+        <v>317.47489588923798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>262.91699999999997</v>
+      </c>
+      <c r="C12" s="6">
+        <v>333.04499999999996</v>
+      </c>
+      <c r="D12" s="6">
+        <v>556.98500000000013</v>
+      </c>
+      <c r="E12" s="6">
+        <v>266.43699999999995</v>
+      </c>
+      <c r="F12" s="6">
+        <v>264.45899999999995</v>
+      </c>
+      <c r="G12" s="6">
+        <v>324.4199999999999</v>
+      </c>
+      <c r="H12" s="6">
+        <v>677.14399999999989</v>
+      </c>
+      <c r="I12" s="6">
+        <v>472.14100000000008</v>
+      </c>
+      <c r="J12" s="6">
+        <v>282.07200000000012</v>
+      </c>
+      <c r="K12" s="6">
+        <v>384.86399999999992</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12">
+        <f>J4-J18</f>
+        <v>426.5390000000001</v>
+      </c>
+      <c r="O12">
+        <f>O40-O41</f>
+        <v>93.258754179107996</v>
+      </c>
+      <c r="P12">
+        <v>-76.742080469936994</v>
+      </c>
+      <c r="Q12">
+        <v>471.526119530004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>229.59900000000002</v>
+      </c>
+      <c r="C13" s="6">
+        <v>297.57500000000005</v>
+      </c>
+      <c r="D13" s="6">
+        <v>505.92999999999989</v>
+      </c>
+      <c r="E13" s="6">
+        <v>252.50499999999997</v>
+      </c>
+      <c r="F13" s="6">
+        <v>208.80099999999999</v>
+      </c>
+      <c r="G13" s="6">
+        <v>253.31900000000005</v>
+      </c>
+      <c r="H13" s="6">
+        <v>644.601</v>
+      </c>
+      <c r="I13" s="6">
+        <v>391.11500000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <v>269.27500000000003</v>
+      </c>
+      <c r="K13" s="6">
+        <v>330.11200000000002</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13">
+        <f>K4-K18</f>
+        <v>293.41199999999992</v>
+      </c>
+      <c r="Q13">
+        <v>378.267365350896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>152.49299999999999</v>
+      </c>
+      <c r="C14" s="6">
+        <v>294.72900000000004</v>
+      </c>
+      <c r="D14" s="6">
+        <v>534.91200000000015</v>
+      </c>
+      <c r="E14" s="6">
+        <v>252.84699999999998</v>
+      </c>
+      <c r="F14" s="6">
+        <v>581.01700000000005</v>
+      </c>
+      <c r="G14" s="6">
+        <v>288.65700000000004</v>
+      </c>
+      <c r="H14" s="6">
+        <v>667.58799999999997</v>
+      </c>
+      <c r="I14" s="6">
+        <v>421.49</v>
+      </c>
+      <c r="J14" s="6">
+        <v>341.07899999999995</v>
+      </c>
+      <c r="K14" s="6">
+        <v>316.48500000000007</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="U14" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>282.04499999999996</v>
+      </c>
+      <c r="C15" s="6">
+        <v>213.60999999999999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>669.38600000000008</v>
+      </c>
+      <c r="E15" s="6">
+        <v>244.38900000000001</v>
+      </c>
+      <c r="F15" s="6">
+        <v>537.41100000000006</v>
+      </c>
+      <c r="G15" s="6">
+        <v>316.56799999999993</v>
+      </c>
+      <c r="H15" s="6">
+        <v>645.38599999999997</v>
+      </c>
+      <c r="I15" s="6">
+        <v>496.23400000000004</v>
+      </c>
+      <c r="J15" s="6">
+        <v>261.34699999999998</v>
+      </c>
+      <c r="K15" s="6">
+        <v>394.03300000000007</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="U15" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3376.46</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3730.3359999999998</v>
+      </c>
+      <c r="D16" s="8">
+        <v>7021.2450000000008</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3391.3059999999996</v>
+      </c>
+      <c r="F16" s="8">
+        <v>4113.8329999999996</v>
+      </c>
+      <c r="G16" s="8">
+        <v>3387.2769999999996</v>
+      </c>
+      <c r="H16" s="8">
+        <v>8097.509</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5252.9660000000003</v>
+      </c>
+      <c r="J16" s="8">
+        <v>3905.2960000000003</v>
+      </c>
+      <c r="K16" s="8">
+        <v>4825.9889999999996</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="U16" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="U17" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>64.875</v>
+      </c>
+      <c r="C18" s="6">
+        <v>68.061999999999983</v>
+      </c>
+      <c r="D18" s="6">
+        <v>222.16899999999998</v>
+      </c>
+      <c r="E18" s="6">
+        <v>85.350999999999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>52.38</v>
+      </c>
+      <c r="G18" s="6">
+        <v>63.415999999999983</v>
+      </c>
+      <c r="H18" s="6">
+        <v>106.05799999999999</v>
+      </c>
+      <c r="I18" s="6">
+        <v>80.919999999999987</v>
+      </c>
+      <c r="J18" s="6">
+        <v>109.13099999999997</v>
+      </c>
+      <c r="K18" s="6">
+        <v>91.373999999999995</v>
+      </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="U18" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6">
+        <v>101.67499999999997</v>
+      </c>
+      <c r="C19" s="6">
+        <v>96.578000000000003</v>
+      </c>
+      <c r="D19" s="6">
+        <v>370.40100000000001</v>
+      </c>
+      <c r="E19" s="6">
+        <v>126.02299999999998</v>
+      </c>
+      <c r="F19" s="6">
+        <v>80.582999999999998</v>
+      </c>
+      <c r="G19" s="6">
+        <v>111.73299999999999</v>
+      </c>
+      <c r="H19" s="6">
+        <v>152.304</v>
+      </c>
+      <c r="I19" s="6">
+        <v>113.61600000000001</v>
+      </c>
+      <c r="J19" s="6">
+        <v>217.82599999999999</v>
+      </c>
+      <c r="K19" s="6">
+        <v>129.13499999999999</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="U19" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6">
+        <v>119.50399999999999</v>
+      </c>
+      <c r="C20" s="6">
+        <v>121.44</v>
+      </c>
+      <c r="D20" s="6">
+        <v>466.81799999999993</v>
+      </c>
+      <c r="E20" s="6">
+        <v>154.94699999999997</v>
+      </c>
+      <c r="F20" s="6">
+        <v>107.56699999999998</v>
+      </c>
+      <c r="G20" s="6">
+        <v>185.50200000000001</v>
+      </c>
+      <c r="H20" s="6">
+        <v>168.24700000000001</v>
+      </c>
+      <c r="I20" s="6">
+        <v>135.96100000000001</v>
+      </c>
+      <c r="J20" s="6">
+        <v>283.38700000000006</v>
+      </c>
+      <c r="K20" s="6">
+        <v>147.71600000000004</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="U20" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6">
+        <v>128.70500000000001</v>
+      </c>
+      <c r="C21" s="6">
+        <v>138.22</v>
+      </c>
+      <c r="D21" s="6">
+        <v>506.53899999999999</v>
+      </c>
+      <c r="E21" s="6">
+        <v>188.00899999999999</v>
+      </c>
+      <c r="F21" s="6">
+        <v>129.08799999999999</v>
+      </c>
+      <c r="G21" s="6">
+        <v>249.62000000000003</v>
+      </c>
+      <c r="H21" s="6">
+        <v>179.16300000000004</v>
+      </c>
+      <c r="I21" s="6">
+        <v>153.74500000000003</v>
+      </c>
+      <c r="J21" s="6">
+        <v>326.00900000000001</v>
+      </c>
+      <c r="K21" s="6">
+        <v>152.04999999999995</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="U21" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6">
+        <v>103.43</v>
+      </c>
+      <c r="C22" s="6">
+        <v>120.44500000000001</v>
+      </c>
+      <c r="D22" s="6">
+        <v>409.55500000000001</v>
+      </c>
+      <c r="E22" s="6">
+        <v>178.89100000000002</v>
+      </c>
+      <c r="F22" s="6">
+        <v>116.2</v>
+      </c>
+      <c r="G22" s="6">
+        <v>228.75600000000003</v>
+      </c>
+      <c r="H22" s="6">
+        <v>150.25200000000001</v>
+      </c>
+      <c r="I22" s="6">
+        <v>131.77800000000002</v>
+      </c>
+      <c r="J22" s="6">
+        <v>300.93700000000007</v>
+      </c>
+      <c r="K22" s="6">
+        <v>130.52199999999999</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="U22" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="6">
+        <v>111.006</v>
+      </c>
+      <c r="C23" s="6">
+        <v>136.43800000000002</v>
+      </c>
+      <c r="D23" s="6">
+        <v>456.90600000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>201.34900000000002</v>
+      </c>
+      <c r="F23" s="6">
+        <v>130.827</v>
+      </c>
+      <c r="G23" s="6">
+        <v>251.40600000000001</v>
+      </c>
+      <c r="H23" s="6">
+        <v>155.68400000000003</v>
+      </c>
+      <c r="I23" s="6">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="J23" s="6">
+        <v>319.82500000000005</v>
+      </c>
+      <c r="K23" s="6">
+        <v>141.303</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="U23" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="6">
+        <v>112.99000000000002</v>
+      </c>
+      <c r="C24" s="6">
+        <v>133.142</v>
+      </c>
+      <c r="D24" s="6">
+        <v>432.70800000000003</v>
+      </c>
+      <c r="E24" s="6">
+        <v>188.85600000000002</v>
+      </c>
+      <c r="F24" s="6">
+        <v>129.11399999999998</v>
+      </c>
+      <c r="G24" s="6">
+        <v>245.78100000000006</v>
+      </c>
+      <c r="H24" s="6">
+        <v>156.32499999999999</v>
+      </c>
+      <c r="I24" s="6">
+        <v>141.29899999999998</v>
+      </c>
+      <c r="J24" s="6">
+        <v>313.95600000000007</v>
+      </c>
+      <c r="K24" s="6">
+        <v>137.828</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6">
+        <v>98.518000000000015</v>
+      </c>
+      <c r="C25" s="6">
+        <v>114.45700000000002</v>
+      </c>
+      <c r="D25" s="6">
+        <v>411.76100000000002</v>
+      </c>
+      <c r="E25" s="6">
+        <v>157.23799999999997</v>
+      </c>
+      <c r="F25" s="6">
+        <v>105.85400000000001</v>
+      </c>
+      <c r="G25" s="6">
+        <v>199.86899999999997</v>
+      </c>
+      <c r="H25" s="6">
+        <v>137.363</v>
+      </c>
+      <c r="I25" s="6">
+        <v>124.30600000000001</v>
+      </c>
+      <c r="J25" s="6">
+        <v>257.80099999999999</v>
+      </c>
+      <c r="K25" s="6">
+        <v>124.499</v>
+      </c>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="6">
+        <v>111.697</v>
+      </c>
+      <c r="C26" s="6">
+        <v>120.01899999999999</v>
+      </c>
+      <c r="D26" s="6">
+        <v>425.90500000000009</v>
+      </c>
+      <c r="E26" s="6">
+        <v>157.94399999999999</v>
+      </c>
+      <c r="F26" s="6">
+        <v>110.45</v>
+      </c>
+      <c r="G26" s="6">
+        <v>202.65599999999998</v>
+      </c>
+      <c r="H26" s="6">
+        <v>153.88999999999999</v>
+      </c>
+      <c r="I26" s="6">
+        <v>133.56999999999996</v>
+      </c>
+      <c r="J26" s="6">
+        <v>279.60700000000003</v>
+      </c>
+      <c r="K26" s="6">
+        <v>135.64100000000002</v>
+      </c>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6">
+        <v>91.993999999999986</v>
+      </c>
+      <c r="C27" s="6">
+        <v>90.7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>356.572</v>
+      </c>
+      <c r="E27" s="6">
+        <v>118.15700000000002</v>
+      </c>
+      <c r="F27" s="6">
+        <v>79.431999999999988</v>
+      </c>
+      <c r="G27" s="6">
+        <v>139.21600000000001</v>
+      </c>
+      <c r="H27" s="6">
+        <v>134.75900000000001</v>
+      </c>
+      <c r="I27" s="6">
+        <v>105.11500000000001</v>
+      </c>
+      <c r="J27" s="6">
+        <v>196.13999999999996</v>
+      </c>
+      <c r="K27" s="6">
+        <v>122.11399999999999</v>
+      </c>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="6">
+        <v>80.479999999999961</v>
+      </c>
+      <c r="C28" s="6">
+        <v>76.384999999999991</v>
+      </c>
+      <c r="D28" s="6">
+        <v>263.3490000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>98.891999999999982</v>
+      </c>
+      <c r="F28" s="6">
+        <v>61.866000000000014</v>
+      </c>
+      <c r="G28" s="6">
+        <v>115.74799999999998</v>
+      </c>
+      <c r="H28" s="6">
+        <v>114.46799999999999</v>
+      </c>
+      <c r="I28" s="6">
+        <v>90.445999999999984</v>
+      </c>
+      <c r="J28" s="6">
+        <v>146.62799999999999</v>
+      </c>
+      <c r="K28" s="6">
+        <v>103.73099999999999</v>
+      </c>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="6">
+        <v>43.441999999999993</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44.253</v>
+      </c>
+      <c r="D29" s="6">
+        <v>155.75900000000001</v>
+      </c>
+      <c r="E29" s="6">
+        <v>61.987999999999985</v>
+      </c>
+      <c r="F29" s="6">
+        <v>33.684999999999995</v>
+      </c>
+      <c r="G29" s="6">
+        <v>66.321999999999989</v>
+      </c>
+      <c r="H29" s="6">
+        <v>69.669000000000011</v>
+      </c>
+      <c r="I29" s="6">
+        <v>57.185999999999986</v>
+      </c>
+      <c r="J29" s="6">
+        <v>75.953000000000003</v>
+      </c>
+      <c r="K29" s="6">
+        <v>60.731999999999985</v>
+      </c>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1168.316</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1260.1389999999999</v>
+      </c>
+      <c r="D30" s="8">
+        <v>4478.442</v>
+      </c>
+      <c r="E30" s="8">
+        <v>1717.6450000000002</v>
+      </c>
+      <c r="F30" s="8">
+        <v>1137.046</v>
+      </c>
+      <c r="G30" s="8">
+        <v>2060.0250000000001</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1678.1820000000002</v>
+      </c>
+      <c r="I30" s="8">
+        <v>1407.0519999999999</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2827.2000000000003</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1476.645</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>2.81E-3</v>
+      </c>
+      <c r="D32">
+        <v>2.81E-2</v>
+      </c>
+      <c r="E32">
+        <v>7.1199999999999996E-3</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>360</v>
+      </c>
+      <c r="O32">
+        <v>359.382062970292</v>
+      </c>
+      <c r="P32">
+        <v>-17.922609860777801</v>
+      </c>
+      <c r="Q32">
+        <v>-355.74412308192501</v>
+      </c>
+      <c r="R32">
+        <v>53.590008744443502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2.97E-3</v>
+      </c>
+      <c r="D33">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="E33">
+        <v>6.7400000000000003E-3</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>360</v>
+      </c>
+      <c r="O33">
+        <v>344.97290016269602</v>
+      </c>
+      <c r="P33">
+        <v>-16.943766267687</v>
+      </c>
+      <c r="Q33">
+        <v>-341.43022219267999</v>
+      </c>
+      <c r="R33">
+        <v>51.696545967849701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>3.4199999999999999E-3</v>
+      </c>
+      <c r="D34">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="E34">
+        <v>8.7500000000000008E-3</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>360</v>
+      </c>
+      <c r="O34">
+        <v>317.44574016586301</v>
+      </c>
+      <c r="P34">
+        <v>-14.742434944442101</v>
+      </c>
+      <c r="Q34">
+        <v>-313.99234629019099</v>
+      </c>
+      <c r="R34">
+        <v>48.401373701162399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>3.3E-3</v>
+      </c>
+      <c r="D35">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="E35">
+        <v>9.5200000000000007E-3</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>360</v>
+      </c>
+      <c r="O35">
+        <v>329.780296468497</v>
+      </c>
+      <c r="P35">
+        <v>-22.8832077603514</v>
+      </c>
+      <c r="Q35">
+        <v>-326.17481128084802</v>
+      </c>
+      <c r="R35">
+        <v>53.069488926414799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>2.99E-3</v>
+      </c>
+      <c r="D36">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="E36">
+        <v>6.8500000000000002E-3</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>360</v>
+      </c>
+      <c r="O36">
+        <v>474.67512024295399</v>
+      </c>
+      <c r="P36">
+        <v>-30.149422976858599</v>
+      </c>
+      <c r="Q36">
+        <v>-467.91159306214701</v>
+      </c>
+      <c r="R36">
+        <v>84.884628973435994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>3.3E-3</v>
+      </c>
+      <c r="D37">
+        <v>0.03</v>
+      </c>
+      <c r="E37">
+        <v>7.2500000000000004E-3</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>360</v>
+      </c>
+      <c r="O37">
+        <v>366.10796298236602</v>
+      </c>
+      <c r="P37">
+        <v>-20.2259466485955</v>
+      </c>
+      <c r="Q37">
+        <v>-361.671786278995</v>
+      </c>
+      <c r="R37">
+        <v>59.829825770153803</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>7.8499999999999993E-3</v>
+      </c>
+      <c r="D38">
+        <v>4.5199999999999997E-2</v>
+      </c>
+      <c r="E38">
+        <v>4.8599999999999997E-3</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>360</v>
+      </c>
+      <c r="O38">
+        <v>472.33644714343302</v>
+      </c>
+      <c r="P38">
+        <v>-30.125195856030398</v>
+      </c>
+      <c r="Q38">
+        <v>-454.752865946486</v>
+      </c>
+      <c r="R38">
+        <v>130.88478440405501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>4.5199999999999997E-3</v>
+      </c>
+      <c r="D39">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="E39">
+        <v>9.8499999999999994E-3</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>360</v>
+      </c>
+      <c r="O39">
+        <v>317.47489588923798</v>
+      </c>
+      <c r="P39">
+        <v>17.7474381846665</v>
+      </c>
+      <c r="Q39">
+        <v>-312.90413606934601</v>
+      </c>
+      <c r="R39">
+        <v>56.199708420196998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="D40">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E40">
+        <v>7.43E-3</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>360</v>
+      </c>
+      <c r="O40">
+        <v>471.526119530004</v>
+      </c>
+      <c r="P40">
+        <v>11.1737040481067</v>
+      </c>
+      <c r="Q40">
+        <v>-462.40484243144698</v>
+      </c>
+      <c r="R40">
+        <v>92.644277325595297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>5.62E-3</v>
+      </c>
+      <c r="D41">
+        <v>5.6099999999999997E-2</v>
+      </c>
+      <c r="E41">
+        <v>8.8599999999999998E-3</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>360</v>
+      </c>
+      <c r="O41">
+        <v>378.267365350896</v>
+      </c>
+      <c r="P41">
+        <v>2.2032880772130201</v>
+      </c>
+      <c r="Q41">
+        <v>-370.225527368705</v>
+      </c>
+      <c r="R41">
+        <v>77.185998542170907</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="D42">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="E42">
+        <v>4.1230000000000003E-2</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>360</v>
+      </c>
+      <c r="O42">
+        <v>14.3471230819257</v>
+      </c>
+      <c r="P42">
+        <v>-3.4855050413656299</v>
+      </c>
+      <c r="Q42">
+        <v>-14.3450028310688</v>
+      </c>
+      <c r="R42">
+        <v>-0.61629245006602995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>5.8E-4</v>
+      </c>
+      <c r="D43">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="E43">
+        <v>7.5819999999999999E-2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>360</v>
+      </c>
+      <c r="O43">
+        <v>104.84722502375099</v>
+      </c>
+      <c r="P43">
+        <v>-13.9507159635669</v>
+      </c>
+      <c r="Q43">
+        <v>-104.782867293294</v>
+      </c>
+      <c r="R43">
+        <v>7.0122932681342496</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="D44">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="E44">
+        <v>3.5599999999999998E-3</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>360</v>
+      </c>
+      <c r="O44">
+        <v>-34.209786416514099</v>
+      </c>
+      <c r="P44">
+        <v>0.27154737606099399</v>
+      </c>
+      <c r="Q44">
+        <v>34.212712695462798</v>
+      </c>
+      <c r="R44">
+        <v>-0.134762001088823</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>1.23E-3</v>
+      </c>
+      <c r="D45">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E45">
+        <v>7.7799999999999996E-3</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>360</v>
+      </c>
+      <c r="O45">
+        <v>23.046098585389</v>
+      </c>
+      <c r="P45">
+        <v>-0.41796054252824899</v>
+      </c>
+      <c r="Q45">
+        <v>-23.039565766354698</v>
+      </c>
+      <c r="R45">
+        <v>0.16046157127437399</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>5.1999999999999995E-4</v>
+      </c>
+      <c r="D46">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="E46">
+        <v>8.7500000000000008E-3</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>360</v>
+      </c>
+      <c r="O46">
+        <v>-15.604841171438499</v>
+      </c>
+      <c r="P46">
+        <v>-0.19704544660092799</v>
+      </c>
+      <c r="Q46">
+        <v>15.606107729647601</v>
+      </c>
+      <c r="R46">
+        <v>-0.572732794483648</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="D47">
+        <v>7.0300000000000001E-2</v>
+      </c>
+      <c r="E47">
+        <v>4.1230000000000003E-2</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>360</v>
+      </c>
+      <c r="O47">
+        <v>151.735678549287</v>
+      </c>
+      <c r="P47">
+        <v>5.03495109295205</v>
+      </c>
+      <c r="Q47">
+        <v>-151.62723039320099</v>
+      </c>
+      <c r="R47">
+        <v>7.0631241683859596</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>5.8E-4</v>
+      </c>
+      <c r="D48">
+        <v>8.8900000000000007E-2</v>
+      </c>
+      <c r="E48">
+        <v>5.5820000000000002E-2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>360</v>
+      </c>
+      <c r="O48">
+        <v>21.453096342636801</v>
+      </c>
+      <c r="P48">
+        <v>-2.7263787843348499</v>
+      </c>
+      <c r="Q48">
+        <v>-21.450426953429002</v>
+      </c>
+      <c r="R48">
+        <v>-2.44646828364057</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D49">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E49">
+        <v>1.026E-2</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>360</v>
+      </c>
+      <c r="O49">
+        <v>-112.45443697595201</v>
+      </c>
+      <c r="P49">
+        <v>11.507547631629</v>
+      </c>
+      <c r="Q49">
+        <v>112.607922903483</v>
+      </c>
+      <c r="R49">
+        <v>-10.9986883563143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D50">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E50">
+        <v>1.026E-2</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>360</v>
+      </c>
+      <c r="O50">
+        <v>-76.742080469936994</v>
+      </c>
+      <c r="P50">
+        <v>7.5220148947757801</v>
+      </c>
+      <c r="Q50">
+        <v>76.813527370487407</v>
+      </c>
+      <c r="R50">
+        <v>-7.8335458892690903</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Expand load data to 30 homes. Some small changes to case file.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="28">
   <si>
     <t>Column Labels</t>
   </si>
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +222,21 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -270,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -288,6 +303,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,7 +669,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,1583 +2493,2073 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="12"/>
+    <col min="14" max="14" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="9.140625" style="12"/>
+    <col min="29" max="29" width="14.7109375" style="12" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Z1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="13">
         <v>40</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="13">
         <v>41</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="13">
         <v>42</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="13">
         <v>43</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="13">
         <v>44</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="13">
         <v>45</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="13">
         <v>46</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="13">
         <v>47</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="13">
         <v>48</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="13">
         <v>49</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="13">
         <v>70</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="13">
         <v>71</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="13">
         <v>72</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="13">
         <v>73</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="13">
         <v>74</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="13">
         <v>75</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="13">
         <v>76</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="13">
         <v>77</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="13">
         <v>78</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="13">
         <v>79</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="Z2" s="2">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>65</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>67</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>68</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>70</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>71</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>72</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="17">
         <v>406.27199999999999</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="17">
         <v>318.98999999999995</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="17">
         <v>675.154</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="17">
         <v>354.26699999999994</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="17">
         <v>558.93599999999981</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="17">
         <v>257.74599999999998</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="17">
         <v>690.98499999999979</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="17">
         <v>527.72899999999993</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="17">
         <v>535.67000000000007</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="17">
         <v>384.78599999999989</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="17">
         <v>4710.5349999999999</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="17">
         <v>750.30500000000006</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="17">
         <v>475.37900000000002</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="17">
         <v>865.04600000000005</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="17">
         <v>349.54500000000002</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="17">
         <v>612.52699999999993</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="17">
         <v>763.84799999999996</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="17">
         <v>632.32500000000005</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="17">
         <v>544.19600000000003</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="17">
         <v>540.55799999999999</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="17">
         <v>1035.6550000000002</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="17">
         <v>6569.384</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="Z4" s="6">
+        <v>422.28899999999999</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>731.08800000000008</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>291.05200000000002</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>551.31700000000001</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>420.64299999999986</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>534.67600000000004</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>750.30500000000006</v>
+      </c>
+      <c r="AG4" s="6">
+        <v>475.37900000000002</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>865.04600000000005</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>349.54500000000002</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>5391.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="17">
         <v>391.24900000000014</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="17">
         <v>271.78699999999992</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="17">
         <v>610.51000000000022</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="17">
         <v>331.23499999999996</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="17">
         <v>409.15500000000009</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="17">
         <v>355.06799999999998</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="17">
         <v>692.18099999999981</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="17">
         <v>432.83100000000007</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="17">
         <v>506.02500000000003</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="17">
         <v>396.22999999999996</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="17">
         <v>4396.2709999999997</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="17">
         <v>675.21800000000007</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="17">
         <v>403.73399999999998</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="17">
         <v>663.072</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="17">
         <v>333.91</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="17">
         <v>512.00699999999995</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="17">
         <v>754.32699999999977</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="17">
         <v>611.33299999999997</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="17">
         <v>517.75</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="17">
         <v>489.7750000000002</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="17">
         <v>833.79700000000014</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="17">
         <v>5794.9230000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="Z5" s="6">
+        <v>355.29699999999997</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>658.81100000000004</v>
+      </c>
+      <c r="AB5" s="6">
+        <v>259.73700000000002</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>635.63499999999999</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>245.74599999999995</v>
+      </c>
+      <c r="AE5" s="6">
+        <v>607.17400000000009</v>
+      </c>
+      <c r="AF5" s="6">
+        <v>675.21800000000007</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>403.73399999999998</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>663.072</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>333.91</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>4838.3339999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="17">
         <v>319.85600000000005</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="17">
         <v>281.54799999999994</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="17">
         <v>537.07299999999998</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="17">
         <v>228.96600000000004</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="17">
         <v>216.82600000000002</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="17">
         <v>296.69999999999993</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="17">
         <v>634.92500000000007</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="17">
         <v>347.27100000000002</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="17">
         <v>314.5089999999999</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="17">
         <v>291.36200000000002</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="17">
         <v>3469.0360000000005</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="17">
         <v>577.39599999999996</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="17">
         <v>340.2709999999999</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="17">
         <v>589.54100000000005</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="17">
         <v>283.036</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="17">
         <v>505.548</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="17">
         <v>618.42800000000011</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="17">
         <v>408.90699999999998</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="17">
         <v>325.94499999999999</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="17">
         <v>366.62</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="17">
         <v>518.25200000000007</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="17">
         <v>4533.9440000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="Z6" s="6">
+        <v>244.14599999999996</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>459.80199999999996</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>196.03800000000004</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>525.45100000000002</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>470.63599999999997</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>562.74499999999989</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>577.39599999999996</v>
+      </c>
+      <c r="AG6" s="6">
+        <v>340.2709999999999</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>589.54100000000005</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>283.036</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>4249.0619999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="17">
         <v>221.238</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="17">
         <v>326.07299999999992</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="17">
         <v>547.10800000000006</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="17">
         <v>229.934</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="17">
         <v>237.36300000000003</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="17">
         <v>275.96299999999997</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="17">
         <v>710.96200000000022</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="17">
         <v>354.30100000000004</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="17">
         <v>326.47699999999998</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="17">
         <v>330.08099999999985</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="17">
         <v>3559.4999999999995</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="17">
         <v>617.60899999999981</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="17">
         <v>305.53399999999993</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="17">
         <v>226.75199999999995</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="17">
         <v>292.87099999999992</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="17">
         <v>492.17700000000002</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="17">
         <v>893.96800000000007</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="17">
         <v>328.92599999999987</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="17">
         <v>297.53299999999996</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="17">
         <v>373.91499999999996</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="17">
         <v>362.27799999999985</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7" s="17">
         <v>4191.5630000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="Z7" s="6">
+        <v>234.58600000000001</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>294.68799999999999</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>114.10700000000003</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>582.13399999999979</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>473.74</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>522.13799999999992</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>617.60899999999981</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>305.53399999999993</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>226.75199999999995</v>
+      </c>
+      <c r="AI7" s="6">
+        <v>292.87099999999992</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>3664.1590000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="17">
         <v>247.71300000000002</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="17">
         <v>400.83600000000001</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="17">
         <v>553.18399999999997</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="17">
         <v>244.37999999999994</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="17">
         <v>193.68400000000005</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="17">
         <v>221.959</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="17">
         <v>660.11999999999978</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="17">
         <v>397.04199999999997</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="17">
         <v>274.30599999999993</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="17">
         <v>377.53799999999995</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="17">
         <v>3570.7619999999997</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="17">
         <v>585.57899999999995</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="17">
         <v>308.80800000000005</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="17">
         <v>202.89299999999997</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="17">
         <v>290.65099999999995</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="17">
         <v>433.45099999999991</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="17">
         <v>941.26700000000017</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="17">
         <v>331.72600000000006</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="17">
         <v>145.02599999999998</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="17">
         <v>446.07800000000003</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8" s="17">
         <v>403.32800000000003</v>
       </c>
-      <c r="X8" s="6">
+      <c r="X8" s="17">
         <v>4088.8070000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="Z8" s="6">
+        <v>236.68999999999997</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>451.702</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>217.87699999999998</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>545.03700000000003</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>531.63699999999994</v>
+      </c>
+      <c r="AE8" s="6">
+        <v>520.96499999999992</v>
+      </c>
+      <c r="AF8" s="6">
+        <v>585.57899999999995</v>
+      </c>
+      <c r="AG8" s="6">
+        <v>308.80800000000005</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>202.89299999999997</v>
+      </c>
+      <c r="AI8" s="6">
+        <v>290.65099999999995</v>
+      </c>
+      <c r="AJ8" s="6">
+        <v>3891.8389999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="17">
         <v>297.50299999999999</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="17">
         <v>365.10000000000008</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="17">
         <v>653.93000000000006</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="17">
         <v>341.09199999999998</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="17">
         <v>339.72799999999995</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="17">
         <v>236.94299999999998</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="17">
         <v>695.90700000000004</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="17">
         <v>387.185</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="17">
         <v>285.101</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="17">
         <v>517.99900000000014</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="17">
         <v>4120.4880000000003</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="17">
         <v>706.90499999999986</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="17">
         <v>326.69699999999995</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="17">
         <v>179.80199999999999</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="17">
         <v>306.29199999999997</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="17">
         <v>408.25999999999993</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="17">
         <v>1047.1130000000003</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="17">
         <v>337.71999999999986</v>
       </c>
-      <c r="U9" s="6">
+      <c r="U9" s="17">
         <v>154.22899999999998</v>
       </c>
-      <c r="V9" s="6">
+      <c r="V9" s="17">
         <v>513.89399999999989</v>
       </c>
-      <c r="W9" s="6">
+      <c r="W9" s="17">
         <v>472.02699999999999</v>
       </c>
-      <c r="X9" s="6">
+      <c r="X9" s="17">
         <v>4452.9389999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="Z9" s="6">
+        <v>233.52400000000003</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>452.221</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>238.70899999999997</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>579.81600000000003</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>605.077</v>
+      </c>
+      <c r="AE9" s="6">
+        <v>594.5569999999999</v>
+      </c>
+      <c r="AF9" s="6">
+        <v>706.90499999999986</v>
+      </c>
+      <c r="AG9" s="6">
+        <v>326.69699999999995</v>
+      </c>
+      <c r="AH9" s="6">
+        <v>179.80199999999999</v>
+      </c>
+      <c r="AI9" s="6">
+        <v>306.29199999999997</v>
+      </c>
+      <c r="AJ9" s="6">
+        <v>4223.5999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="17">
         <v>325.54700000000003</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="17">
         <v>348.14399999999995</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="17">
         <v>633.2969999999998</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="17">
         <v>404.13799999999998</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="17">
         <v>289.24399999999997</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="17">
         <v>258.39699999999999</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="17">
         <v>731.07199999999989</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="17">
         <v>577.52899999999977</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="17">
         <v>283.29200000000003</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="17">
         <v>717.49099999999976</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="17">
         <v>4568.1509999999989</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="17">
         <v>757.46800000000007</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="17">
         <v>410.41600000000011</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="17">
         <v>188.42</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="17">
         <v>387.02399999999994</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="17">
         <v>331.834</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="17">
         <v>794.53099999999995</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="17">
         <v>365.262</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="17">
         <v>212.88</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="17">
         <v>530.54</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="17">
         <v>556.7320000000002</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10" s="17">
         <v>4535.1070000000009</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="Z10" s="6">
+        <v>282.57299999999998</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>660.7439999999998</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>274.34099999999995</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>568.45700000000011</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>610.58800000000019</v>
+      </c>
+      <c r="AE10" s="6">
+        <v>621.21900000000016</v>
+      </c>
+      <c r="AF10" s="6">
+        <v>757.46800000000007</v>
+      </c>
+      <c r="AG10" s="6">
+        <v>410.41600000000011</v>
+      </c>
+      <c r="AH10" s="6">
+        <v>188.42</v>
+      </c>
+      <c r="AI10" s="6">
+        <v>387.02399999999994</v>
+      </c>
+      <c r="AJ10" s="6">
+        <v>4761.2500000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="17">
         <v>240.02799999999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="17">
         <v>278.899</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="17">
         <v>543.77600000000007</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="17">
         <v>241.11599999999996</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="17">
         <v>277.209</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="17">
         <v>301.53699999999998</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="17">
         <v>646.63799999999992</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="17">
         <v>448.09800000000007</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="17">
         <v>226.14300000000006</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="17">
         <v>385.00799999999998</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="17">
         <v>3588.4519999999998</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="17">
         <v>561.92199999999991</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="17">
         <v>377.6160000000001</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="17">
         <v>180.827</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="17">
         <v>280.07100000000008</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="17">
         <v>340.65400000000005</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="17">
         <v>886.77499999999986</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="17">
         <v>289.52900000000005</v>
       </c>
-      <c r="U11" s="6">
+      <c r="U11" s="17">
         <v>259.5150000000001</v>
       </c>
-      <c r="V11" s="6">
+      <c r="V11" s="17">
         <v>369.423</v>
       </c>
-      <c r="W11" s="6">
+      <c r="W11" s="17">
         <v>314.25399999999996</v>
       </c>
-      <c r="X11" s="6">
+      <c r="X11" s="17">
         <v>3860.5859999999993</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="Z11" s="6">
+        <v>271.22399999999999</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>492.36500000000001</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>243.84199999999998</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>553.97100000000012</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>531.20800000000008</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>505.84199999999998</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>561.92199999999991</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>377.6160000000001</v>
+      </c>
+      <c r="AH11" s="6">
+        <v>180.827</v>
+      </c>
+      <c r="AI11" s="6">
+        <v>280.07100000000008</v>
+      </c>
+      <c r="AJ11" s="6">
+        <v>3998.8879999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="17">
         <v>262.91699999999997</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="17">
         <v>333.04499999999996</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="17">
         <v>556.98500000000013</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="17">
         <v>266.43699999999995</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="17">
         <v>264.45899999999995</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="17">
         <v>324.4199999999999</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="17">
         <v>677.14399999999989</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="17">
         <v>472.14100000000008</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="17">
         <v>282.07200000000012</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="17">
         <v>384.86399999999992</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="17">
         <v>3824.4839999999999</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="17">
         <v>675.10800000000006</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="17">
         <v>416.53399999999993</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="17">
         <v>200.37800000000007</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="17">
         <v>292.74699999999996</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="17">
         <v>354.21100000000013</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="17">
         <v>986.81800000000032</v>
       </c>
-      <c r="T12" s="6">
+      <c r="T12" s="17">
         <v>324.43299999999999</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="17">
         <v>293.423</v>
       </c>
-      <c r="V12" s="6">
+      <c r="V12" s="17">
         <v>492.92199999999991</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12" s="17">
         <v>393.30499999999989</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12" s="17">
         <v>4429.8790000000008</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="Z12" s="6">
+        <v>266.48300000000006</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>519.71300000000008</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>302.24599999999987</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>579.80599999999993</v>
+      </c>
+      <c r="AD12" s="6">
+        <v>607.38600000000008</v>
+      </c>
+      <c r="AE12" s="6">
+        <v>579.4620000000001</v>
+      </c>
+      <c r="AF12" s="6">
+        <v>675.10800000000006</v>
+      </c>
+      <c r="AG12" s="6">
+        <v>416.53399999999993</v>
+      </c>
+      <c r="AH12" s="6">
+        <v>200.37800000000007</v>
+      </c>
+      <c r="AI12" s="6">
+        <v>292.74699999999996</v>
+      </c>
+      <c r="AJ12" s="6">
+        <v>4439.8630000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="17">
         <v>229.59900000000002</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="17">
         <v>297.57500000000005</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="17">
         <v>505.92999999999989</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="17">
         <v>252.50499999999997</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="17">
         <v>208.80099999999999</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="17">
         <v>253.31900000000005</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="17">
         <v>644.601</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="17">
         <v>391.11500000000001</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="17">
         <v>269.27500000000003</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="17">
         <v>330.11200000000002</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="17">
         <v>3382.8319999999999</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="17">
         <v>520.13099999999997</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="17">
         <v>470.43400000000003</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="17">
         <v>237.86199999999999</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="17">
         <v>318.95699999999999</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="17">
         <v>412.42900000000003</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="17">
         <v>656.51600000000019</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="17">
         <v>360.36699999999996</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="17">
         <v>205.851</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="17">
         <v>480.70799999999997</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="17">
         <v>344.57099999999991</v>
       </c>
-      <c r="X13" s="6">
+      <c r="X13" s="17">
         <v>4007.826</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="Z13" s="6">
+        <v>237.02500000000001</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>307.37900000000002</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>248.27700000000004</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>431.54599999999994</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>531.05200000000013</v>
+      </c>
+      <c r="AE13" s="6">
+        <v>613.66700000000003</v>
+      </c>
+      <c r="AF13" s="6">
+        <v>520.13099999999997</v>
+      </c>
+      <c r="AG13" s="6">
+        <v>470.43400000000003</v>
+      </c>
+      <c r="AH13" s="6">
+        <v>237.86199999999999</v>
+      </c>
+      <c r="AI13" s="6">
+        <v>318.95699999999999</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>3916.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="17">
         <v>152.49299999999999</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="17">
         <v>294.72900000000004</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="17">
         <v>534.91200000000015</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="17">
         <v>252.84699999999998</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="17">
         <v>581.01700000000005</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="17">
         <v>288.65700000000004</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="17">
         <v>667.58799999999997</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="17">
         <v>421.49</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="17">
         <v>341.07899999999995</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="17">
         <v>316.48500000000007</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="17">
         <v>3851.297</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="17">
         <v>613.77</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="17">
         <v>480.87599999999998</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="17">
         <v>612.755</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="17">
         <v>322.15600000000001</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="17">
         <v>575.75500000000011</v>
       </c>
-      <c r="S14" s="6">
+      <c r="S14" s="17">
         <v>635.25099999999975</v>
       </c>
-      <c r="T14" s="6">
+      <c r="T14" s="17">
         <v>516.07800000000009</v>
       </c>
-      <c r="U14" s="6">
+      <c r="U14" s="17">
         <v>282.916</v>
       </c>
-      <c r="V14" s="6">
+      <c r="V14" s="17">
         <v>572.75</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W14" s="17">
         <v>554.29399999999976</v>
       </c>
-      <c r="X14" s="6">
+      <c r="X14" s="17">
         <v>5166.6009999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="Z14" s="6">
+        <v>299.56000000000012</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>606.78700000000015</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>297.72199999999998</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>586.61399999999992</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>296.96199999999982</v>
+      </c>
+      <c r="AE14" s="6">
+        <v>522.32799999999986</v>
+      </c>
+      <c r="AF14" s="6">
+        <v>613.77</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>480.87599999999998</v>
+      </c>
+      <c r="AH14" s="6">
+        <v>612.755</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>322.15600000000001</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>4639.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="17">
         <v>282.04499999999996</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="17">
         <v>213.60999999999999</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="17">
         <v>669.38600000000008</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="17">
         <v>244.38900000000001</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="17">
         <v>537.41100000000006</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="17">
         <v>316.56799999999993</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="17">
         <v>645.38599999999997</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="17">
         <v>496.23400000000004</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="17">
         <v>261.34699999999998</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="17">
         <v>394.03300000000007</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="17">
         <v>4060.4090000000001</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="17">
         <v>721.53199999999993</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="17">
         <v>511.83499999999992</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="17">
         <v>703.19900000000007</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="17">
         <v>364.64300000000003</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="17">
         <v>794.42600000000004</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="17">
         <v>622.15300000000002</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="17">
         <v>598.69900000000007</v>
       </c>
-      <c r="U15" s="6">
+      <c r="U15" s="17">
         <v>428.50799999999992</v>
       </c>
-      <c r="V15" s="6">
+      <c r="V15" s="17">
         <v>586.85</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="17">
         <v>690.64300000000026</v>
       </c>
-      <c r="X15" s="6">
+      <c r="X15" s="17">
         <v>6022.4879999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="Z15" s="6">
+        <v>413.79</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>797.12200000000007</v>
+      </c>
+      <c r="AB15" s="6">
+        <v>273.84600000000006</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>573.39100000000008</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>458.65599999999984</v>
+      </c>
+      <c r="AE15" s="6">
+        <v>499.92</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>721.53199999999993</v>
+      </c>
+      <c r="AG15" s="6">
+        <v>511.83499999999992</v>
+      </c>
+      <c r="AH15" s="6">
+        <v>703.19900000000007</v>
+      </c>
+      <c r="AI15" s="6">
+        <v>364.64300000000003</v>
+      </c>
+      <c r="AJ15" s="6">
+        <v>5317.9340000000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="19">
         <v>3376.46</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="19">
         <v>3730.3359999999998</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="19">
         <v>7021.2450000000008</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="19">
         <v>3391.3059999999996</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="19">
         <v>4113.8329999999996</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="19">
         <v>3387.2769999999996</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="19">
         <v>8097.509</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="19">
         <v>5252.9660000000003</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="19">
         <v>3905.2960000000003</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="19">
         <v>4825.9889999999996</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="19">
         <v>47102.216999999997</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="19">
         <v>7762.9430000000002</v>
       </c>
-      <c r="O16" s="8">
+      <c r="O16" s="19">
         <v>4828.134</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="19">
         <v>4850.5470000000005</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="Q16" s="19">
         <v>3821.9029999999993</v>
       </c>
-      <c r="R16" s="8">
+      <c r="R16" s="19">
         <v>5773.2790000000005</v>
       </c>
-      <c r="S16" s="8">
+      <c r="S16" s="19">
         <v>9600.9950000000008</v>
       </c>
-      <c r="T16" s="8">
+      <c r="T16" s="19">
         <v>5105.3050000000003</v>
       </c>
-      <c r="U16" s="8">
+      <c r="U16" s="19">
         <v>3667.7719999999995</v>
       </c>
-      <c r="V16" s="8">
+      <c r="V16" s="19">
         <v>5764.0329999999994</v>
       </c>
-      <c r="W16" s="8">
+      <c r="W16" s="19">
         <v>6479.1360000000004</v>
       </c>
-      <c r="X16" s="8">
+      <c r="X16" s="19">
         <v>57654.046999999999</v>
       </c>
+      <c r="Z16" s="8">
+        <v>3497.1870000000004</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>6432.4220000000005</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>2957.7939999999994</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>6713.1749999999993</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>5783.3309999999992</v>
+      </c>
+      <c r="AE16" s="8">
+        <v>6684.6930000000002</v>
+      </c>
+      <c r="AF16" s="8">
+        <v>7762.9430000000002</v>
+      </c>
+      <c r="AG16" s="8">
+        <v>4828.134</v>
+      </c>
+      <c r="AH16" s="8">
+        <v>4850.5470000000005</v>
+      </c>
+      <c r="AI16" s="8">
+        <v>3821.9029999999993</v>
+      </c>
+      <c r="AJ16" s="8">
+        <v>53332.129000000001</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="17">
         <v>64.875</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="17">
         <v>68.061999999999983</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="17">
         <v>222.16899999999998</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="17">
         <v>85.350999999999999</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="17">
         <v>52.38</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="17">
         <v>63.415999999999983</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="17">
         <v>106.05799999999999</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="17">
         <v>80.919999999999987</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="17">
         <v>109.13099999999997</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="17">
         <v>91.373999999999995</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="17">
         <v>943.73599999999988</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="17">
         <v>101.67499999999997</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="17">
         <v>96.578000000000003</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="17">
         <v>370.40100000000001</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="17">
         <v>126.02299999999998</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="17">
         <v>80.582999999999998</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="17">
         <v>111.73299999999999</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="17">
         <v>152.304</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="17">
         <v>113.61600000000001</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="17">
         <v>217.82599999999999</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="17">
         <v>129.13499999999999</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="17">
         <v>1499.874</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="17">
         <v>119.50399999999999</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="17">
         <v>121.44</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="17">
         <v>466.81799999999993</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="17">
         <v>154.94699999999997</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="17">
         <v>107.56699999999998</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="17">
         <v>185.50200000000001</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="17">
         <v>168.24700000000001</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="17">
         <v>135.96100000000001</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="17">
         <v>283.38700000000006</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="17">
         <v>147.71600000000004</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="17">
         <v>1891.0890000000002</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="17">
         <v>128.70500000000001</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="17">
         <v>138.22</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="17">
         <v>506.53899999999999</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="17">
         <v>188.00899999999999</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="17">
         <v>129.08799999999999</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="17">
         <v>249.62000000000003</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="17">
         <v>179.16300000000004</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="17">
         <v>153.74500000000003</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="17">
         <v>326.00900000000001</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="17">
         <v>152.04999999999995</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="17">
         <v>2151.1480000000001</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="17">
         <v>103.43</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="17">
         <v>120.44500000000001</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="17">
         <v>409.55500000000001</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="17">
         <v>178.89100000000002</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="17">
         <v>116.2</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="17">
         <v>228.75600000000003</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="17">
         <v>150.25200000000001</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="17">
         <v>131.77800000000002</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="17">
         <v>300.93700000000007</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="17">
         <v>130.52199999999999</v>
       </c>
-      <c r="L22" s="6">
+      <c r="L22" s="17">
         <v>1870.7660000000003</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="17">
         <v>111.006</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="17">
         <v>136.43800000000002</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="17">
         <v>456.90600000000001</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="17">
         <v>201.34900000000002</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="17">
         <v>130.827</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="17">
         <v>251.40600000000001</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="17">
         <v>155.68400000000003</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="17">
         <v>139.11000000000001</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="17">
         <v>319.82500000000005</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="17">
         <v>141.303</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="17">
         <v>2043.8540000000003</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="17">
         <v>112.99000000000002</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="17">
         <v>133.142</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="17">
         <v>432.70800000000003</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="17">
         <v>188.85600000000002</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="17">
         <v>129.11399999999998</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="17">
         <v>245.78100000000006</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="17">
         <v>156.32499999999999</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="17">
         <v>141.29899999999998</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="17">
         <v>313.95600000000007</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="17">
         <v>137.828</v>
       </c>
-      <c r="L24" s="6">
+      <c r="L24" s="17">
         <v>1991.999</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="17">
         <v>98.518000000000015</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="17">
         <v>114.45700000000002</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="17">
         <v>411.76100000000002</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="17">
         <v>157.23799999999997</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="17">
         <v>105.85400000000001</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="17">
         <v>199.86899999999997</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="17">
         <v>137.363</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="17">
         <v>124.30600000000001</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="17">
         <v>257.80099999999999</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="17">
         <v>124.499</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="17">
         <v>1731.6660000000002</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="17">
         <v>111.697</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="17">
         <v>120.01899999999999</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="17">
         <v>425.90500000000009</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="17">
         <v>157.94399999999999</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="17">
         <v>110.45</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="17">
         <v>202.65599999999998</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="17">
         <v>153.88999999999999</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="17">
         <v>133.56999999999996</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="17">
         <v>279.60700000000003</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="17">
         <v>135.64100000000002</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L26" s="17">
         <v>1831.3790000000001</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="17">
         <v>91.993999999999986</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="17">
         <v>90.7</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="17">
         <v>356.572</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="17">
         <v>118.15700000000002</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="17">
         <v>79.431999999999988</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="17">
         <v>139.21600000000001</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="17">
         <v>134.75900000000001</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="17">
         <v>105.11500000000001</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="17">
         <v>196.13999999999996</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="17">
         <v>122.11399999999999</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="17">
         <v>1434.1990000000001</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="17">
         <v>80.479999999999961</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="17">
         <v>76.384999999999991</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="17">
         <v>263.3490000000001</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="17">
         <v>98.891999999999982</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="17">
         <v>61.866000000000014</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="17">
         <v>115.74799999999998</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="17">
         <v>114.46799999999999</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="17">
         <v>90.445999999999984</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="17">
         <v>146.62799999999999</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="17">
         <v>103.73099999999999</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L28" s="17">
         <v>1151.9929999999999</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="17">
         <v>43.441999999999993</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="17">
         <v>44.253</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="17">
         <v>155.75900000000001</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="17">
         <v>61.987999999999985</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="17">
         <v>33.684999999999995</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="17">
         <v>66.321999999999989</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="17">
         <v>69.669000000000011</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="17">
         <v>57.185999999999986</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="17">
         <v>75.953000000000003</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="17">
         <v>60.731999999999985</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L29" s="17">
         <v>668.98900000000003</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="19">
         <v>1168.316</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="19">
         <v>1260.1389999999999</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="19">
         <v>4478.442</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="19">
         <v>1717.6450000000002</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="19">
         <v>1137.046</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="19">
         <v>2060.0250000000001</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="19">
         <v>1678.1820000000002</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="19">
         <v>1407.0519999999999</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="19">
         <v>2827.2000000000003</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="19">
         <v>1476.645</v>
       </c>
-      <c r="L30" s="8">
+      <c r="L30" s="19">
         <v>19210.692000000003</v>
       </c>
     </row>
@@ -4053,7 +4573,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U14:U23"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4194,7 +4714,7 @@
         <v>341.39699999999999</v>
       </c>
       <c r="O4">
-        <f>O32-O33</f>
+        <f t="shared" ref="O4:O12" si="0">O32-O33</f>
         <v>14.409162807595976</v>
       </c>
       <c r="P4">
@@ -4245,7 +4765,7 @@
         <v>250.92799999999997</v>
       </c>
       <c r="O5">
-        <f>O33-O34</f>
+        <f t="shared" si="0"/>
         <v>27.527159996833007</v>
       </c>
       <c r="P5">
@@ -4296,7 +4816,7 @@
         <v>452.98500000000001</v>
       </c>
       <c r="O6">
-        <f>O34-O35</f>
+        <f t="shared" si="0"/>
         <v>-12.334556302633985</v>
       </c>
       <c r="P6">
@@ -4347,7 +4867,7 @@
         <v>268.91599999999994</v>
       </c>
       <c r="O7">
-        <f>O35-O36</f>
+        <f t="shared" si="0"/>
         <v>-144.894823774457</v>
       </c>
       <c r="P7">
@@ -4398,7 +4918,7 @@
         <v>506.55599999999981</v>
       </c>
       <c r="O8">
-        <f>O36-O37</f>
+        <f t="shared" si="0"/>
         <v>108.56715726058798</v>
       </c>
       <c r="P8">
@@ -4449,7 +4969,7 @@
         <v>194.32999999999998</v>
       </c>
       <c r="O9">
-        <f>O37-O38</f>
+        <f t="shared" si="0"/>
         <v>-106.228484161067</v>
       </c>
       <c r="P9">
@@ -4500,7 +5020,7 @@
         <v>584.92699999999979</v>
       </c>
       <c r="O10">
-        <f>O38-O39</f>
+        <f t="shared" si="0"/>
         <v>154.86155125419504</v>
       </c>
       <c r="P10">
@@ -4551,7 +5071,7 @@
         <v>446.80899999999997</v>
       </c>
       <c r="O11">
-        <f>O39-O40</f>
+        <f t="shared" si="0"/>
         <v>-154.05122364076601</v>
       </c>
       <c r="P11">
@@ -4602,7 +5122,7 @@
         <v>426.5390000000001</v>
       </c>
       <c r="O12">
-        <f>O40-O41</f>
+        <f t="shared" si="0"/>
         <v>93.258754179107996</v>
       </c>
       <c r="P12">

</xml_diff>

<commit_message>
Adds 100 home branch modification for further research
Also modifies 30 homes file name to make room for other 30 home system.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly data sample" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Monthly 10 homes 2" sheetId="3" r:id="rId3"/>
     <sheet name="Monthly 100 homes" sheetId="5" r:id="rId4"/>
     <sheet name="40-49 extra calc" sheetId="4" r:id="rId5"/>
+    <sheet name="Monthly 10 homes 3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="30">
   <si>
     <t>Column Labels</t>
   </si>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t>delta MG</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -719,7 +726,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -752,6 +759,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2903,7 +2914,7 @@
   <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="B1" sqref="B1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,10 +4988,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX30"/>
+  <dimension ref="A1:CX54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13621,6 +13632,598 @@
         <v>226854.93899999998</v>
       </c>
     </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="2">
+        <v>40</v>
+      </c>
+      <c r="C38" s="2">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2">
+        <v>42</v>
+      </c>
+      <c r="E38" s="2">
+        <v>43</v>
+      </c>
+      <c r="F38" s="2">
+        <v>44</v>
+      </c>
+      <c r="G38" s="2">
+        <v>45</v>
+      </c>
+      <c r="H38" s="2">
+        <v>46</v>
+      </c>
+      <c r="I38" s="2">
+        <v>47</v>
+      </c>
+      <c r="J38" s="2">
+        <v>48</v>
+      </c>
+      <c r="K38" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="21">
+        <v>1883.8310000000001</v>
+      </c>
+      <c r="C40" s="21">
+        <v>1964.3339999999998</v>
+      </c>
+      <c r="D40" s="21">
+        <v>3576.9590000000007</v>
+      </c>
+      <c r="E40" s="21">
+        <v>1729.8739999999998</v>
+      </c>
+      <c r="F40" s="21">
+        <v>1955.692</v>
+      </c>
+      <c r="G40" s="21">
+        <v>1644.3789999999999</v>
+      </c>
+      <c r="H40" s="21">
+        <v>4085.08</v>
+      </c>
+      <c r="I40" s="21">
+        <v>2446.3589999999999</v>
+      </c>
+      <c r="J40" s="21">
+        <v>2242.0880000000002</v>
+      </c>
+      <c r="K40" s="21">
+        <v>2297.9960000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="6">
+        <v>406.27199999999999</v>
+      </c>
+      <c r="C41" s="6">
+        <v>318.98999999999995</v>
+      </c>
+      <c r="D41" s="6">
+        <v>675.154</v>
+      </c>
+      <c r="E41" s="6">
+        <v>354.26699999999994</v>
+      </c>
+      <c r="F41" s="6">
+        <v>558.93599999999981</v>
+      </c>
+      <c r="G41" s="6">
+        <v>257.74599999999998</v>
+      </c>
+      <c r="H41" s="6">
+        <v>690.98499999999979</v>
+      </c>
+      <c r="I41" s="6">
+        <v>527.72899999999993</v>
+      </c>
+      <c r="J41" s="6">
+        <v>535.67000000000007</v>
+      </c>
+      <c r="K41" s="6">
+        <v>384.78599999999989</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="6">
+        <v>391.24900000000014</v>
+      </c>
+      <c r="C42" s="6">
+        <v>271.78699999999992</v>
+      </c>
+      <c r="D42" s="6">
+        <v>610.51000000000022</v>
+      </c>
+      <c r="E42" s="6">
+        <v>331.23499999999996</v>
+      </c>
+      <c r="F42" s="6">
+        <v>409.15500000000009</v>
+      </c>
+      <c r="G42" s="6">
+        <v>355.06799999999998</v>
+      </c>
+      <c r="H42" s="6">
+        <v>692.18099999999981</v>
+      </c>
+      <c r="I42" s="6">
+        <v>432.83100000000007</v>
+      </c>
+      <c r="J42" s="6">
+        <v>506.02500000000003</v>
+      </c>
+      <c r="K42" s="6">
+        <v>396.22999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="6">
+        <v>319.85600000000005</v>
+      </c>
+      <c r="C43" s="6">
+        <v>281.54799999999994</v>
+      </c>
+      <c r="D43" s="6">
+        <v>537.07299999999998</v>
+      </c>
+      <c r="E43" s="6">
+        <v>228.96600000000004</v>
+      </c>
+      <c r="F43" s="6">
+        <v>216.82600000000002</v>
+      </c>
+      <c r="G43" s="6">
+        <v>296.69999999999993</v>
+      </c>
+      <c r="H43" s="6">
+        <v>634.92500000000007</v>
+      </c>
+      <c r="I43" s="6">
+        <v>347.27100000000002</v>
+      </c>
+      <c r="J43" s="6">
+        <v>314.5089999999999</v>
+      </c>
+      <c r="K43" s="6">
+        <v>291.36200000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="6">
+        <v>221.238</v>
+      </c>
+      <c r="C44" s="6">
+        <v>326.07299999999992</v>
+      </c>
+      <c r="D44" s="6">
+        <v>547.10800000000006</v>
+      </c>
+      <c r="E44" s="6">
+        <v>229.934</v>
+      </c>
+      <c r="F44" s="6">
+        <v>237.36300000000003</v>
+      </c>
+      <c r="G44" s="6">
+        <v>275.96299999999997</v>
+      </c>
+      <c r="H44" s="6">
+        <v>710.96200000000022</v>
+      </c>
+      <c r="I44" s="6">
+        <v>354.30100000000004</v>
+      </c>
+      <c r="J44" s="6">
+        <v>326.47699999999998</v>
+      </c>
+      <c r="K44" s="6">
+        <v>330.08099999999985</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="6">
+        <v>247.71300000000002</v>
+      </c>
+      <c r="C45" s="6">
+        <v>400.83600000000001</v>
+      </c>
+      <c r="D45" s="6">
+        <v>553.18399999999997</v>
+      </c>
+      <c r="E45" s="6">
+        <v>244.37999999999994</v>
+      </c>
+      <c r="F45" s="6">
+        <v>193.68400000000005</v>
+      </c>
+      <c r="G45" s="6">
+        <v>221.959</v>
+      </c>
+      <c r="H45" s="6">
+        <v>660.11999999999978</v>
+      </c>
+      <c r="I45" s="6">
+        <v>397.04199999999997</v>
+      </c>
+      <c r="J45" s="6">
+        <v>274.30599999999993</v>
+      </c>
+      <c r="K45" s="6">
+        <v>377.53799999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="6">
+        <v>297.50299999999999</v>
+      </c>
+      <c r="C46" s="6">
+        <v>365.10000000000008</v>
+      </c>
+      <c r="D46" s="6">
+        <v>653.93000000000006</v>
+      </c>
+      <c r="E46" s="6">
+        <v>341.09199999999998</v>
+      </c>
+      <c r="F46" s="6">
+        <v>339.72799999999995</v>
+      </c>
+      <c r="G46" s="6">
+        <v>236.94299999999998</v>
+      </c>
+      <c r="H46" s="6">
+        <v>695.90700000000004</v>
+      </c>
+      <c r="I46" s="6">
+        <v>387.185</v>
+      </c>
+      <c r="J46" s="6">
+        <v>285.101</v>
+      </c>
+      <c r="K46" s="6">
+        <v>517.99900000000014</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="21">
+        <v>1492.6289999999999</v>
+      </c>
+      <c r="C47" s="21">
+        <v>1766.002</v>
+      </c>
+      <c r="D47" s="21">
+        <v>3444.2860000000001</v>
+      </c>
+      <c r="E47" s="21">
+        <v>1661.4319999999998</v>
+      </c>
+      <c r="F47" s="21">
+        <v>2158.1410000000001</v>
+      </c>
+      <c r="G47" s="21">
+        <v>1742.8979999999999</v>
+      </c>
+      <c r="H47" s="21">
+        <v>4012.4289999999996</v>
+      </c>
+      <c r="I47" s="21">
+        <v>2806.607</v>
+      </c>
+      <c r="J47" s="21">
+        <v>1663.2080000000001</v>
+      </c>
+      <c r="K47" s="21">
+        <v>2527.9929999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="6">
+        <v>325.54700000000003</v>
+      </c>
+      <c r="C48" s="6">
+        <v>348.14399999999995</v>
+      </c>
+      <c r="D48" s="6">
+        <v>633.2969999999998</v>
+      </c>
+      <c r="E48" s="6">
+        <v>404.13799999999998</v>
+      </c>
+      <c r="F48" s="6">
+        <v>289.24399999999997</v>
+      </c>
+      <c r="G48" s="6">
+        <v>258.39699999999999</v>
+      </c>
+      <c r="H48" s="6">
+        <v>731.07199999999989</v>
+      </c>
+      <c r="I48" s="6">
+        <v>577.52899999999977</v>
+      </c>
+      <c r="J48" s="6">
+        <v>283.29200000000003</v>
+      </c>
+      <c r="K48" s="6">
+        <v>717.49099999999976</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="6">
+        <v>240.02799999999999</v>
+      </c>
+      <c r="C49" s="6">
+        <v>278.899</v>
+      </c>
+      <c r="D49" s="6">
+        <v>543.77600000000007</v>
+      </c>
+      <c r="E49" s="6">
+        <v>241.11599999999996</v>
+      </c>
+      <c r="F49" s="6">
+        <v>277.209</v>
+      </c>
+      <c r="G49" s="6">
+        <v>301.53699999999998</v>
+      </c>
+      <c r="H49" s="6">
+        <v>646.63799999999992</v>
+      </c>
+      <c r="I49" s="6">
+        <v>448.09800000000007</v>
+      </c>
+      <c r="J49" s="6">
+        <v>226.14300000000006</v>
+      </c>
+      <c r="K49" s="6">
+        <v>385.00799999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="6">
+        <v>262.91699999999997</v>
+      </c>
+      <c r="C50" s="6">
+        <v>333.04499999999996</v>
+      </c>
+      <c r="D50" s="6">
+        <v>556.98500000000013</v>
+      </c>
+      <c r="E50" s="6">
+        <v>266.43699999999995</v>
+      </c>
+      <c r="F50" s="6">
+        <v>264.45899999999995</v>
+      </c>
+      <c r="G50" s="6">
+        <v>324.4199999999999</v>
+      </c>
+      <c r="H50" s="6">
+        <v>677.14399999999989</v>
+      </c>
+      <c r="I50" s="6">
+        <v>472.14100000000008</v>
+      </c>
+      <c r="J50" s="6">
+        <v>282.07200000000012</v>
+      </c>
+      <c r="K50" s="6">
+        <v>384.86399999999992</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="6">
+        <v>229.59900000000002</v>
+      </c>
+      <c r="C51" s="6">
+        <v>297.57500000000005</v>
+      </c>
+      <c r="D51" s="6">
+        <v>505.92999999999989</v>
+      </c>
+      <c r="E51" s="6">
+        <v>252.50499999999997</v>
+      </c>
+      <c r="F51" s="6">
+        <v>208.80099999999999</v>
+      </c>
+      <c r="G51" s="6">
+        <v>253.31900000000005</v>
+      </c>
+      <c r="H51" s="6">
+        <v>644.601</v>
+      </c>
+      <c r="I51" s="6">
+        <v>391.11500000000001</v>
+      </c>
+      <c r="J51" s="6">
+        <v>269.27500000000003</v>
+      </c>
+      <c r="K51" s="6">
+        <v>330.11200000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="6">
+        <v>152.49299999999999</v>
+      </c>
+      <c r="C52" s="6">
+        <v>294.72900000000004</v>
+      </c>
+      <c r="D52" s="6">
+        <v>534.91200000000015</v>
+      </c>
+      <c r="E52" s="6">
+        <v>252.84699999999998</v>
+      </c>
+      <c r="F52" s="6">
+        <v>581.01700000000005</v>
+      </c>
+      <c r="G52" s="6">
+        <v>288.65700000000004</v>
+      </c>
+      <c r="H52" s="6">
+        <v>667.58799999999997</v>
+      </c>
+      <c r="I52" s="6">
+        <v>421.49</v>
+      </c>
+      <c r="J52" s="6">
+        <v>341.07899999999995</v>
+      </c>
+      <c r="K52" s="6">
+        <v>316.48500000000007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="6">
+        <v>282.04499999999996</v>
+      </c>
+      <c r="C53" s="6">
+        <v>213.60999999999999</v>
+      </c>
+      <c r="D53" s="6">
+        <v>669.38600000000008</v>
+      </c>
+      <c r="E53" s="6">
+        <v>244.38900000000001</v>
+      </c>
+      <c r="F53" s="6">
+        <v>537.41100000000006</v>
+      </c>
+      <c r="G53" s="6">
+        <v>316.56799999999993</v>
+      </c>
+      <c r="H53" s="6">
+        <v>645.38599999999997</v>
+      </c>
+      <c r="I53" s="6">
+        <v>496.23400000000004</v>
+      </c>
+      <c r="J53" s="6">
+        <v>261.34699999999998</v>
+      </c>
+      <c r="K53" s="6">
+        <v>394.03300000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="8">
+        <v>3376.46</v>
+      </c>
+      <c r="C54" s="8">
+        <v>3730.3359999999998</v>
+      </c>
+      <c r="D54" s="8">
+        <v>7021.2450000000008</v>
+      </c>
+      <c r="E54" s="8">
+        <v>3391.3059999999996</v>
+      </c>
+      <c r="F54" s="8">
+        <v>4113.8329999999996</v>
+      </c>
+      <c r="G54" s="8">
+        <v>3387.2769999999996</v>
+      </c>
+      <c r="H54" s="8">
+        <v>8097.509</v>
+      </c>
+      <c r="I54" s="8">
+        <v>5252.9660000000003</v>
+      </c>
+      <c r="J54" s="8">
+        <v>3905.2960000000003</v>
+      </c>
+      <c r="K54" s="8">
+        <v>4825.9889999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16114,4 +16717,2081 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="12"/>
+    <col min="14" max="14" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="9.140625" style="12"/>
+    <col min="29" max="29" width="14.7109375" style="12" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="N1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Z1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2">
+        <v>63</v>
+      </c>
+      <c r="F2" s="2">
+        <v>64</v>
+      </c>
+      <c r="G2" s="2">
+        <v>65</v>
+      </c>
+      <c r="H2" s="2">
+        <v>66</v>
+      </c>
+      <c r="I2" s="2">
+        <v>67</v>
+      </c>
+      <c r="J2" s="2">
+        <v>68</v>
+      </c>
+      <c r="K2" s="2">
+        <v>69</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="13">
+        <v>70</v>
+      </c>
+      <c r="O2" s="13">
+        <v>71</v>
+      </c>
+      <c r="P2" s="13">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>73</v>
+      </c>
+      <c r="R2" s="13">
+        <v>74</v>
+      </c>
+      <c r="S2" s="13">
+        <v>75</v>
+      </c>
+      <c r="T2" s="13">
+        <v>76</v>
+      </c>
+      <c r="U2" s="13">
+        <v>77</v>
+      </c>
+      <c r="V2" s="13">
+        <v>78</v>
+      </c>
+      <c r="W2" s="13">
+        <v>79</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>65</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>67</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>68</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>70</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>71</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>72</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>511.0030000000001</v>
+      </c>
+      <c r="C4" s="6">
+        <v>641.41499999999985</v>
+      </c>
+      <c r="D4" s="6">
+        <v>890.92899999999975</v>
+      </c>
+      <c r="E4" s="6">
+        <v>724.91200000000003</v>
+      </c>
+      <c r="F4" s="6">
+        <v>422.28899999999999</v>
+      </c>
+      <c r="G4" s="6">
+        <v>731.08800000000008</v>
+      </c>
+      <c r="H4" s="6">
+        <v>291.05200000000002</v>
+      </c>
+      <c r="I4" s="6">
+        <v>551.31700000000001</v>
+      </c>
+      <c r="J4" s="6">
+        <v>420.64299999999986</v>
+      </c>
+      <c r="K4" s="6">
+        <v>534.67600000000004</v>
+      </c>
+      <c r="L4" s="6">
+        <v>5719.3240000000005</v>
+      </c>
+      <c r="N4" s="17">
+        <v>750.30500000000006</v>
+      </c>
+      <c r="O4" s="17">
+        <v>475.37900000000002</v>
+      </c>
+      <c r="P4" s="17">
+        <v>865.04600000000005</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>349.54500000000002</v>
+      </c>
+      <c r="R4" s="17">
+        <v>612.52699999999993</v>
+      </c>
+      <c r="S4" s="17">
+        <v>763.84799999999996</v>
+      </c>
+      <c r="T4" s="17">
+        <v>632.32500000000005</v>
+      </c>
+      <c r="U4" s="17">
+        <v>544.19600000000003</v>
+      </c>
+      <c r="V4" s="17">
+        <v>540.55799999999999</v>
+      </c>
+      <c r="W4" s="17">
+        <v>1035.6550000000002</v>
+      </c>
+      <c r="X4" s="17">
+        <v>6569.384</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>422.28899999999999</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>731.08800000000008</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>291.05200000000002</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>551.31700000000001</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>420.64299999999986</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>534.67600000000004</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>750.30500000000006</v>
+      </c>
+      <c r="AG4" s="6">
+        <v>475.37900000000002</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>865.04600000000005</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>349.54500000000002</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>5391.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>447.7600000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>587.93800000000022</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1152.2399999999998</v>
+      </c>
+      <c r="E5" s="6">
+        <v>684.81700000000001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>355.29699999999997</v>
+      </c>
+      <c r="G5" s="6">
+        <v>658.81100000000004</v>
+      </c>
+      <c r="H5" s="6">
+        <v>259.73700000000002</v>
+      </c>
+      <c r="I5" s="6">
+        <v>635.63499999999999</v>
+      </c>
+      <c r="J5" s="6">
+        <v>245.74599999999995</v>
+      </c>
+      <c r="K5" s="6">
+        <v>607.17400000000009</v>
+      </c>
+      <c r="L5" s="6">
+        <v>5635.1550000000007</v>
+      </c>
+      <c r="N5" s="17">
+        <v>675.21800000000007</v>
+      </c>
+      <c r="O5" s="17">
+        <v>403.73399999999998</v>
+      </c>
+      <c r="P5" s="17">
+        <v>663.072</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>333.91</v>
+      </c>
+      <c r="R5" s="17">
+        <v>512.00699999999995</v>
+      </c>
+      <c r="S5" s="17">
+        <v>754.32699999999977</v>
+      </c>
+      <c r="T5" s="17">
+        <v>611.33299999999997</v>
+      </c>
+      <c r="U5" s="17">
+        <v>517.75</v>
+      </c>
+      <c r="V5" s="17">
+        <v>489.7750000000002</v>
+      </c>
+      <c r="W5" s="17">
+        <v>833.79700000000014</v>
+      </c>
+      <c r="X5" s="17">
+        <v>5794.9230000000007</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>355.29699999999997</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>658.81100000000004</v>
+      </c>
+      <c r="AB5" s="6">
+        <v>259.73700000000002</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>635.63499999999999</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>245.74599999999995</v>
+      </c>
+      <c r="AE5" s="6">
+        <v>607.17400000000009</v>
+      </c>
+      <c r="AF5" s="6">
+        <v>675.21800000000007</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>403.73399999999998</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>663.072</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>333.91</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>4838.3339999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>304.48699999999997</v>
+      </c>
+      <c r="C6" s="6">
+        <v>484.17500000000007</v>
+      </c>
+      <c r="D6" s="6">
+        <v>799.38900000000012</v>
+      </c>
+      <c r="E6" s="6">
+        <v>612.93199999999979</v>
+      </c>
+      <c r="F6" s="6">
+        <v>244.14599999999996</v>
+      </c>
+      <c r="G6" s="6">
+        <v>459.80199999999996</v>
+      </c>
+      <c r="H6" s="6">
+        <v>196.03800000000004</v>
+      </c>
+      <c r="I6" s="6">
+        <v>525.45100000000002</v>
+      </c>
+      <c r="J6" s="6">
+        <v>470.63599999999997</v>
+      </c>
+      <c r="K6" s="6">
+        <v>562.74499999999989</v>
+      </c>
+      <c r="L6" s="6">
+        <v>4659.8010000000004</v>
+      </c>
+      <c r="N6" s="17">
+        <v>577.39599999999996</v>
+      </c>
+      <c r="O6" s="17">
+        <v>340.2709999999999</v>
+      </c>
+      <c r="P6" s="17">
+        <v>589.54100000000005</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>283.036</v>
+      </c>
+      <c r="R6" s="17">
+        <v>505.548</v>
+      </c>
+      <c r="S6" s="17">
+        <v>618.42800000000011</v>
+      </c>
+      <c r="T6" s="17">
+        <v>408.90699999999998</v>
+      </c>
+      <c r="U6" s="17">
+        <v>325.94499999999999</v>
+      </c>
+      <c r="V6" s="17">
+        <v>366.62</v>
+      </c>
+      <c r="W6" s="17">
+        <v>518.25200000000007</v>
+      </c>
+      <c r="X6" s="17">
+        <v>4533.9440000000004</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>244.14599999999996</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>459.80199999999996</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>196.03800000000004</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>525.45100000000002</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>470.63599999999997</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>562.74499999999989</v>
+      </c>
+      <c r="AF6" s="6">
+        <v>577.39599999999996</v>
+      </c>
+      <c r="AG6" s="6">
+        <v>340.2709999999999</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>589.54100000000005</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>283.036</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>4249.0619999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>280.23299999999995</v>
+      </c>
+      <c r="C7" s="6">
+        <v>466.78200000000004</v>
+      </c>
+      <c r="D7" s="6">
+        <v>968.07300000000009</v>
+      </c>
+      <c r="E7" s="6">
+        <v>563.22900000000004</v>
+      </c>
+      <c r="F7" s="6">
+        <v>234.58600000000001</v>
+      </c>
+      <c r="G7" s="6">
+        <v>294.68799999999999</v>
+      </c>
+      <c r="H7" s="6">
+        <v>114.10700000000003</v>
+      </c>
+      <c r="I7" s="6">
+        <v>582.13399999999979</v>
+      </c>
+      <c r="J7" s="6">
+        <v>473.74</v>
+      </c>
+      <c r="K7" s="6">
+        <v>522.13799999999992</v>
+      </c>
+      <c r="L7" s="6">
+        <v>4499.71</v>
+      </c>
+      <c r="N7" s="17">
+        <v>617.60899999999981</v>
+      </c>
+      <c r="O7" s="17">
+        <v>305.53399999999993</v>
+      </c>
+      <c r="P7" s="17">
+        <v>226.75199999999995</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>292.87099999999992</v>
+      </c>
+      <c r="R7" s="17">
+        <v>492.17700000000002</v>
+      </c>
+      <c r="S7" s="17">
+        <v>893.96800000000007</v>
+      </c>
+      <c r="T7" s="17">
+        <v>328.92599999999987</v>
+      </c>
+      <c r="U7" s="17">
+        <v>297.53299999999996</v>
+      </c>
+      <c r="V7" s="17">
+        <v>373.91499999999996</v>
+      </c>
+      <c r="W7" s="17">
+        <v>362.27799999999985</v>
+      </c>
+      <c r="X7" s="17">
+        <v>4191.5630000000001</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>234.58600000000001</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>294.68799999999999</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>114.10700000000003</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>582.13399999999979</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>473.74</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>522.13799999999992</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>617.60899999999981</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>305.53399999999993</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>226.75199999999995</v>
+      </c>
+      <c r="AI7" s="6">
+        <v>292.87099999999992</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>3664.1590000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>290.00500000000005</v>
+      </c>
+      <c r="C8" s="6">
+        <v>477.35299999999995</v>
+      </c>
+      <c r="D8" s="6">
+        <v>899.16799999999978</v>
+      </c>
+      <c r="E8" s="6">
+        <v>493.36600000000004</v>
+      </c>
+      <c r="F8" s="6">
+        <v>236.68999999999997</v>
+      </c>
+      <c r="G8" s="6">
+        <v>451.702</v>
+      </c>
+      <c r="H8" s="6">
+        <v>217.87699999999998</v>
+      </c>
+      <c r="I8" s="6">
+        <v>545.03700000000003</v>
+      </c>
+      <c r="J8" s="6">
+        <v>531.63699999999994</v>
+      </c>
+      <c r="K8" s="6">
+        <v>520.96499999999992</v>
+      </c>
+      <c r="L8" s="6">
+        <v>4663.7999999999993</v>
+      </c>
+      <c r="N8" s="17">
+        <v>585.57899999999995</v>
+      </c>
+      <c r="O8" s="17">
+        <v>308.80800000000005</v>
+      </c>
+      <c r="P8" s="17">
+        <v>202.89299999999997</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>290.65099999999995</v>
+      </c>
+      <c r="R8" s="17">
+        <v>433.45099999999991</v>
+      </c>
+      <c r="S8" s="17">
+        <v>941.26700000000017</v>
+      </c>
+      <c r="T8" s="17">
+        <v>331.72600000000006</v>
+      </c>
+      <c r="U8" s="17">
+        <v>145.02599999999998</v>
+      </c>
+      <c r="V8" s="17">
+        <v>446.07800000000003</v>
+      </c>
+      <c r="W8" s="17">
+        <v>403.32800000000003</v>
+      </c>
+      <c r="X8" s="17">
+        <v>4088.8070000000002</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>236.68999999999997</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>451.702</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>217.87699999999998</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>545.03700000000003</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>531.63699999999994</v>
+      </c>
+      <c r="AE8" s="6">
+        <v>520.96499999999992</v>
+      </c>
+      <c r="AF8" s="6">
+        <v>585.57899999999995</v>
+      </c>
+      <c r="AG8" s="6">
+        <v>308.80800000000005</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>202.89299999999997</v>
+      </c>
+      <c r="AI8" s="6">
+        <v>290.65099999999995</v>
+      </c>
+      <c r="AJ8" s="6">
+        <v>3891.8389999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>298.36800000000005</v>
+      </c>
+      <c r="C9" s="6">
+        <v>614.29300000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>762.79299999999989</v>
+      </c>
+      <c r="E9" s="6">
+        <v>466.01399999999995</v>
+      </c>
+      <c r="F9" s="6">
+        <v>233.52400000000003</v>
+      </c>
+      <c r="G9" s="6">
+        <v>452.221</v>
+      </c>
+      <c r="H9" s="6">
+        <v>238.70899999999997</v>
+      </c>
+      <c r="I9" s="6">
+        <v>579.81600000000003</v>
+      </c>
+      <c r="J9" s="6">
+        <v>605.077</v>
+      </c>
+      <c r="K9" s="6">
+        <v>594.5569999999999</v>
+      </c>
+      <c r="L9" s="6">
+        <v>4845.3719999999994</v>
+      </c>
+      <c r="N9" s="17">
+        <v>706.90499999999986</v>
+      </c>
+      <c r="O9" s="17">
+        <v>326.69699999999995</v>
+      </c>
+      <c r="P9" s="17">
+        <v>179.80199999999999</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>306.29199999999997</v>
+      </c>
+      <c r="R9" s="17">
+        <v>408.25999999999993</v>
+      </c>
+      <c r="S9" s="17">
+        <v>1047.1130000000003</v>
+      </c>
+      <c r="T9" s="17">
+        <v>337.71999999999986</v>
+      </c>
+      <c r="U9" s="17">
+        <v>154.22899999999998</v>
+      </c>
+      <c r="V9" s="17">
+        <v>513.89399999999989</v>
+      </c>
+      <c r="W9" s="17">
+        <v>472.02699999999999</v>
+      </c>
+      <c r="X9" s="17">
+        <v>4452.9389999999994</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>233.52400000000003</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>452.221</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>238.70899999999997</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>579.81600000000003</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>605.077</v>
+      </c>
+      <c r="AE9" s="6">
+        <v>594.5569999999999</v>
+      </c>
+      <c r="AF9" s="6">
+        <v>706.90499999999986</v>
+      </c>
+      <c r="AG9" s="6">
+        <v>326.69699999999995</v>
+      </c>
+      <c r="AH9" s="6">
+        <v>179.80199999999999</v>
+      </c>
+      <c r="AI9" s="6">
+        <v>306.29199999999997</v>
+      </c>
+      <c r="AJ9" s="6">
+        <v>4223.5999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>379.12099999999992</v>
+      </c>
+      <c r="C10" s="6">
+        <v>736.36900000000003</v>
+      </c>
+      <c r="D10" s="6">
+        <v>779.66200000000003</v>
+      </c>
+      <c r="E10" s="6">
+        <v>513.55599999999993</v>
+      </c>
+      <c r="F10" s="6">
+        <v>282.57299999999998</v>
+      </c>
+      <c r="G10" s="6">
+        <v>660.7439999999998</v>
+      </c>
+      <c r="H10" s="6">
+        <v>274.34099999999995</v>
+      </c>
+      <c r="I10" s="6">
+        <v>568.45700000000011</v>
+      </c>
+      <c r="J10" s="6">
+        <v>610.58800000000019</v>
+      </c>
+      <c r="K10" s="6">
+        <v>621.21900000000016</v>
+      </c>
+      <c r="L10" s="6">
+        <v>5426.63</v>
+      </c>
+      <c r="N10" s="17">
+        <v>757.46800000000007</v>
+      </c>
+      <c r="O10" s="17">
+        <v>410.41600000000011</v>
+      </c>
+      <c r="P10" s="17">
+        <v>188.42</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>387.02399999999994</v>
+      </c>
+      <c r="R10" s="17">
+        <v>331.834</v>
+      </c>
+      <c r="S10" s="17">
+        <v>794.53099999999995</v>
+      </c>
+      <c r="T10" s="17">
+        <v>365.262</v>
+      </c>
+      <c r="U10" s="17">
+        <v>212.88</v>
+      </c>
+      <c r="V10" s="17">
+        <v>530.54</v>
+      </c>
+      <c r="W10" s="17">
+        <v>556.7320000000002</v>
+      </c>
+      <c r="X10" s="17">
+        <v>4535.1070000000009</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>282.57299999999998</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>660.7439999999998</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>274.34099999999995</v>
+      </c>
+      <c r="AC10" s="6">
+        <v>568.45700000000011</v>
+      </c>
+      <c r="AD10" s="6">
+        <v>610.58800000000019</v>
+      </c>
+      <c r="AE10" s="6">
+        <v>621.21900000000016</v>
+      </c>
+      <c r="AF10" s="6">
+        <v>757.46800000000007</v>
+      </c>
+      <c r="AG10" s="6">
+        <v>410.41600000000011</v>
+      </c>
+      <c r="AH10" s="6">
+        <v>188.42</v>
+      </c>
+      <c r="AI10" s="6">
+        <v>387.02399999999994</v>
+      </c>
+      <c r="AJ10" s="6">
+        <v>4761.2500000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>241.19900000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>562.4190000000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>758.80100000000004</v>
+      </c>
+      <c r="E11" s="6">
+        <v>403.74499999999989</v>
+      </c>
+      <c r="F11" s="6">
+        <v>271.22399999999999</v>
+      </c>
+      <c r="G11" s="6">
+        <v>492.36500000000001</v>
+      </c>
+      <c r="H11" s="6">
+        <v>243.84199999999998</v>
+      </c>
+      <c r="I11" s="6">
+        <v>553.97100000000012</v>
+      </c>
+      <c r="J11" s="6">
+        <v>531.20800000000008</v>
+      </c>
+      <c r="K11" s="6">
+        <v>505.84199999999998</v>
+      </c>
+      <c r="L11" s="6">
+        <v>4564.6160000000009</v>
+      </c>
+      <c r="N11" s="17">
+        <v>561.92199999999991</v>
+      </c>
+      <c r="O11" s="17">
+        <v>377.6160000000001</v>
+      </c>
+      <c r="P11" s="17">
+        <v>180.827</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>280.07100000000008</v>
+      </c>
+      <c r="R11" s="17">
+        <v>340.65400000000005</v>
+      </c>
+      <c r="S11" s="17">
+        <v>886.77499999999986</v>
+      </c>
+      <c r="T11" s="17">
+        <v>289.52900000000005</v>
+      </c>
+      <c r="U11" s="17">
+        <v>259.5150000000001</v>
+      </c>
+      <c r="V11" s="17">
+        <v>369.423</v>
+      </c>
+      <c r="W11" s="17">
+        <v>314.25399999999996</v>
+      </c>
+      <c r="X11" s="17">
+        <v>3860.5859999999993</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>271.22399999999999</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>492.36500000000001</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>243.84199999999998</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>553.97100000000012</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>531.20800000000008</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>505.84199999999998</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>561.92199999999991</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>377.6160000000001</v>
+      </c>
+      <c r="AH11" s="6">
+        <v>180.827</v>
+      </c>
+      <c r="AI11" s="6">
+        <v>280.07100000000008</v>
+      </c>
+      <c r="AJ11" s="6">
+        <v>3998.8879999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>250.30500000000001</v>
+      </c>
+      <c r="C12" s="6">
+        <v>576.35100000000011</v>
+      </c>
+      <c r="D12" s="6">
+        <v>879.10100000000011</v>
+      </c>
+      <c r="E12" s="6">
+        <v>434.67599999999982</v>
+      </c>
+      <c r="F12" s="6">
+        <v>266.48300000000006</v>
+      </c>
+      <c r="G12" s="6">
+        <v>519.71300000000008</v>
+      </c>
+      <c r="H12" s="6">
+        <v>302.24599999999987</v>
+      </c>
+      <c r="I12" s="6">
+        <v>579.80599999999993</v>
+      </c>
+      <c r="J12" s="6">
+        <v>607.38600000000008</v>
+      </c>
+      <c r="K12" s="6">
+        <v>579.4620000000001</v>
+      </c>
+      <c r="L12" s="6">
+        <v>4995.5290000000005</v>
+      </c>
+      <c r="N12" s="17">
+        <v>675.10800000000006</v>
+      </c>
+      <c r="O12" s="17">
+        <v>416.53399999999993</v>
+      </c>
+      <c r="P12" s="17">
+        <v>200.37800000000007</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>292.74699999999996</v>
+      </c>
+      <c r="R12" s="17">
+        <v>354.21100000000013</v>
+      </c>
+      <c r="S12" s="17">
+        <v>986.81800000000032</v>
+      </c>
+      <c r="T12" s="17">
+        <v>324.43299999999999</v>
+      </c>
+      <c r="U12" s="17">
+        <v>293.423</v>
+      </c>
+      <c r="V12" s="17">
+        <v>492.92199999999991</v>
+      </c>
+      <c r="W12" s="17">
+        <v>393.30499999999989</v>
+      </c>
+      <c r="X12" s="17">
+        <v>4429.8790000000008</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>266.48300000000006</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>519.71300000000008</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>302.24599999999987</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>579.80599999999993</v>
+      </c>
+      <c r="AD12" s="6">
+        <v>607.38600000000008</v>
+      </c>
+      <c r="AE12" s="6">
+        <v>579.4620000000001</v>
+      </c>
+      <c r="AF12" s="6">
+        <v>675.10800000000006</v>
+      </c>
+      <c r="AG12" s="6">
+        <v>416.53399999999993</v>
+      </c>
+      <c r="AH12" s="6">
+        <v>200.37800000000007</v>
+      </c>
+      <c r="AI12" s="6">
+        <v>292.74699999999996</v>
+      </c>
+      <c r="AJ12" s="6">
+        <v>4439.8630000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>238.60400000000001</v>
+      </c>
+      <c r="C13" s="6">
+        <v>486.24100000000004</v>
+      </c>
+      <c r="D13" s="6">
+        <v>820.4290000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>498.49999999999989</v>
+      </c>
+      <c r="F13" s="6">
+        <v>237.02500000000001</v>
+      </c>
+      <c r="G13" s="6">
+        <v>307.37900000000002</v>
+      </c>
+      <c r="H13" s="6">
+        <v>248.27700000000004</v>
+      </c>
+      <c r="I13" s="6">
+        <v>431.54599999999994</v>
+      </c>
+      <c r="J13" s="6">
+        <v>531.05200000000013</v>
+      </c>
+      <c r="K13" s="6">
+        <v>613.66700000000003</v>
+      </c>
+      <c r="L13" s="6">
+        <v>4412.72</v>
+      </c>
+      <c r="N13" s="17">
+        <v>520.13099999999997</v>
+      </c>
+      <c r="O13" s="17">
+        <v>470.43400000000003</v>
+      </c>
+      <c r="P13" s="17">
+        <v>237.86199999999999</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>318.95699999999999</v>
+      </c>
+      <c r="R13" s="17">
+        <v>412.42900000000003</v>
+      </c>
+      <c r="S13" s="17">
+        <v>656.51600000000019</v>
+      </c>
+      <c r="T13" s="17">
+        <v>360.36699999999996</v>
+      </c>
+      <c r="U13" s="17">
+        <v>205.851</v>
+      </c>
+      <c r="V13" s="17">
+        <v>480.70799999999997</v>
+      </c>
+      <c r="W13" s="17">
+        <v>344.57099999999991</v>
+      </c>
+      <c r="X13" s="17">
+        <v>4007.826</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>237.02500000000001</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>307.37900000000002</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>248.27700000000004</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>431.54599999999994</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>531.05200000000013</v>
+      </c>
+      <c r="AE13" s="6">
+        <v>613.66700000000003</v>
+      </c>
+      <c r="AF13" s="6">
+        <v>520.13099999999997</v>
+      </c>
+      <c r="AG13" s="6">
+        <v>470.43400000000003</v>
+      </c>
+      <c r="AH13" s="6">
+        <v>237.86199999999999</v>
+      </c>
+      <c r="AI13" s="6">
+        <v>318.95699999999999</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>3916.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>231.73</v>
+      </c>
+      <c r="C14" s="6">
+        <v>478.62199999999984</v>
+      </c>
+      <c r="D14" s="6">
+        <v>755.42700000000002</v>
+      </c>
+      <c r="E14" s="6">
+        <v>595.38199999999995</v>
+      </c>
+      <c r="F14" s="6">
+        <v>299.56000000000012</v>
+      </c>
+      <c r="G14" s="6">
+        <v>606.78700000000015</v>
+      </c>
+      <c r="H14" s="6">
+        <v>297.72199999999998</v>
+      </c>
+      <c r="I14" s="6">
+        <v>586.61399999999992</v>
+      </c>
+      <c r="J14" s="6">
+        <v>296.96199999999982</v>
+      </c>
+      <c r="K14" s="6">
+        <v>522.32799999999986</v>
+      </c>
+      <c r="L14" s="6">
+        <v>4671.134</v>
+      </c>
+      <c r="N14" s="17">
+        <v>613.77</v>
+      </c>
+      <c r="O14" s="17">
+        <v>480.87599999999998</v>
+      </c>
+      <c r="P14" s="17">
+        <v>612.755</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>322.15600000000001</v>
+      </c>
+      <c r="R14" s="17">
+        <v>575.75500000000011</v>
+      </c>
+      <c r="S14" s="17">
+        <v>635.25099999999975</v>
+      </c>
+      <c r="T14" s="17">
+        <v>516.07800000000009</v>
+      </c>
+      <c r="U14" s="17">
+        <v>282.916</v>
+      </c>
+      <c r="V14" s="17">
+        <v>572.75</v>
+      </c>
+      <c r="W14" s="17">
+        <v>554.29399999999976</v>
+      </c>
+      <c r="X14" s="17">
+        <v>5166.6009999999997</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>299.56000000000012</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>606.78700000000015</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>297.72199999999998</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>586.61399999999992</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>296.96199999999982</v>
+      </c>
+      <c r="AE14" s="6">
+        <v>522.32799999999986</v>
+      </c>
+      <c r="AF14" s="6">
+        <v>613.77</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>480.87599999999998</v>
+      </c>
+      <c r="AH14" s="6">
+        <v>612.755</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>322.15600000000001</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>4639.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>341.07000000000005</v>
+      </c>
+      <c r="C15" s="6">
+        <v>468.03600000000006</v>
+      </c>
+      <c r="D15" s="6">
+        <v>764.37199999999996</v>
+      </c>
+      <c r="E15" s="6">
+        <v>589.71500000000015</v>
+      </c>
+      <c r="F15" s="6">
+        <v>413.79</v>
+      </c>
+      <c r="G15" s="6">
+        <v>797.12200000000007</v>
+      </c>
+      <c r="H15" s="6">
+        <v>273.84600000000006</v>
+      </c>
+      <c r="I15" s="6">
+        <v>573.39100000000008</v>
+      </c>
+      <c r="J15" s="6">
+        <v>458.65599999999984</v>
+      </c>
+      <c r="K15" s="6">
+        <v>499.92</v>
+      </c>
+      <c r="L15" s="6">
+        <v>5179.9180000000006</v>
+      </c>
+      <c r="N15" s="17">
+        <v>721.53199999999993</v>
+      </c>
+      <c r="O15" s="17">
+        <v>511.83499999999992</v>
+      </c>
+      <c r="P15" s="17">
+        <v>703.19900000000007</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>364.64300000000003</v>
+      </c>
+      <c r="R15" s="17">
+        <v>794.42600000000004</v>
+      </c>
+      <c r="S15" s="17">
+        <v>622.15300000000002</v>
+      </c>
+      <c r="T15" s="17">
+        <v>598.69900000000007</v>
+      </c>
+      <c r="U15" s="17">
+        <v>428.50799999999992</v>
+      </c>
+      <c r="V15" s="17">
+        <v>586.85</v>
+      </c>
+      <c r="W15" s="17">
+        <v>690.64300000000026</v>
+      </c>
+      <c r="X15" s="17">
+        <v>6022.4879999999994</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>413.79</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>797.12200000000007</v>
+      </c>
+      <c r="AB15" s="6">
+        <v>273.84600000000006</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>573.39100000000008</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>458.65599999999984</v>
+      </c>
+      <c r="AE15" s="6">
+        <v>499.92</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>721.53199999999993</v>
+      </c>
+      <c r="AG15" s="6">
+        <v>511.83499999999992</v>
+      </c>
+      <c r="AH15" s="6">
+        <v>703.19900000000007</v>
+      </c>
+      <c r="AI15" s="6">
+        <v>364.64300000000003</v>
+      </c>
+      <c r="AJ15" s="6">
+        <v>5317.9340000000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3813.8850000000002</v>
+      </c>
+      <c r="C16" s="8">
+        <v>6579.9940000000006</v>
+      </c>
+      <c r="D16" s="8">
+        <v>10230.383999999998</v>
+      </c>
+      <c r="E16" s="8">
+        <v>6580.8439999999991</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3497.1870000000004</v>
+      </c>
+      <c r="G16" s="8">
+        <v>6432.4220000000005</v>
+      </c>
+      <c r="H16" s="8">
+        <v>2957.7939999999994</v>
+      </c>
+      <c r="I16" s="8">
+        <v>6713.1749999999993</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5783.3309999999992</v>
+      </c>
+      <c r="K16" s="8">
+        <v>6684.6930000000002</v>
+      </c>
+      <c r="L16" s="8">
+        <v>59273.709000000003</v>
+      </c>
+      <c r="N16" s="19">
+        <v>7762.9430000000002</v>
+      </c>
+      <c r="O16" s="19">
+        <v>4828.134</v>
+      </c>
+      <c r="P16" s="19">
+        <v>4850.5470000000005</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>3821.9029999999993</v>
+      </c>
+      <c r="R16" s="19">
+        <v>5773.2790000000005</v>
+      </c>
+      <c r="S16" s="19">
+        <v>9600.9950000000008</v>
+      </c>
+      <c r="T16" s="19">
+        <v>5105.3050000000003</v>
+      </c>
+      <c r="U16" s="19">
+        <v>3667.7719999999995</v>
+      </c>
+      <c r="V16" s="19">
+        <v>5764.0329999999994</v>
+      </c>
+      <c r="W16" s="19">
+        <v>6479.1360000000004</v>
+      </c>
+      <c r="X16" s="19">
+        <v>57654.046999999999</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>3497.1870000000004</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>6432.4220000000005</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>2957.7939999999994</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>6713.1749999999993</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>5783.3309999999992</v>
+      </c>
+      <c r="AE16" s="8">
+        <v>6684.6930000000002</v>
+      </c>
+      <c r="AF16" s="8">
+        <v>7762.9430000000002</v>
+      </c>
+      <c r="AG16" s="8">
+        <v>4828.134</v>
+      </c>
+      <c r="AH16" s="8">
+        <v>4850.5470000000005</v>
+      </c>
+      <c r="AI16" s="8">
+        <v>3821.9029999999993</v>
+      </c>
+      <c r="AJ16" s="8">
+        <v>53332.129000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="17">
+        <v>64.875</v>
+      </c>
+      <c r="C18" s="17">
+        <v>68.061999999999983</v>
+      </c>
+      <c r="D18" s="17">
+        <v>222.16899999999998</v>
+      </c>
+      <c r="E18" s="17">
+        <v>85.350999999999999</v>
+      </c>
+      <c r="F18" s="17">
+        <v>52.38</v>
+      </c>
+      <c r="G18" s="17">
+        <v>63.415999999999983</v>
+      </c>
+      <c r="H18" s="17">
+        <v>106.05799999999999</v>
+      </c>
+      <c r="I18" s="17">
+        <v>80.919999999999987</v>
+      </c>
+      <c r="J18" s="17">
+        <v>109.13099999999997</v>
+      </c>
+      <c r="K18" s="17">
+        <v>91.373999999999995</v>
+      </c>
+      <c r="L18" s="17">
+        <v>943.73599999999988</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="17">
+        <v>101.67499999999997</v>
+      </c>
+      <c r="C19" s="17">
+        <v>96.578000000000003</v>
+      </c>
+      <c r="D19" s="17">
+        <v>370.40100000000001</v>
+      </c>
+      <c r="E19" s="17">
+        <v>126.02299999999998</v>
+      </c>
+      <c r="F19" s="17">
+        <v>80.582999999999998</v>
+      </c>
+      <c r="G19" s="17">
+        <v>111.73299999999999</v>
+      </c>
+      <c r="H19" s="17">
+        <v>152.304</v>
+      </c>
+      <c r="I19" s="17">
+        <v>113.61600000000001</v>
+      </c>
+      <c r="J19" s="17">
+        <v>217.82599999999999</v>
+      </c>
+      <c r="K19" s="17">
+        <v>129.13499999999999</v>
+      </c>
+      <c r="L19" s="17">
+        <v>1499.874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="17">
+        <v>119.50399999999999</v>
+      </c>
+      <c r="C20" s="17">
+        <v>121.44</v>
+      </c>
+      <c r="D20" s="17">
+        <v>466.81799999999993</v>
+      </c>
+      <c r="E20" s="17">
+        <v>154.94699999999997</v>
+      </c>
+      <c r="F20" s="17">
+        <v>107.56699999999998</v>
+      </c>
+      <c r="G20" s="17">
+        <v>185.50200000000001</v>
+      </c>
+      <c r="H20" s="17">
+        <v>168.24700000000001</v>
+      </c>
+      <c r="I20" s="17">
+        <v>135.96100000000001</v>
+      </c>
+      <c r="J20" s="17">
+        <v>283.38700000000006</v>
+      </c>
+      <c r="K20" s="17">
+        <v>147.71600000000004</v>
+      </c>
+      <c r="L20" s="17">
+        <v>1891.0890000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="17">
+        <v>128.70500000000001</v>
+      </c>
+      <c r="C21" s="17">
+        <v>138.22</v>
+      </c>
+      <c r="D21" s="17">
+        <v>506.53899999999999</v>
+      </c>
+      <c r="E21" s="17">
+        <v>188.00899999999999</v>
+      </c>
+      <c r="F21" s="17">
+        <v>129.08799999999999</v>
+      </c>
+      <c r="G21" s="17">
+        <v>249.62000000000003</v>
+      </c>
+      <c r="H21" s="17">
+        <v>179.16300000000004</v>
+      </c>
+      <c r="I21" s="17">
+        <v>153.74500000000003</v>
+      </c>
+      <c r="J21" s="17">
+        <v>326.00900000000001</v>
+      </c>
+      <c r="K21" s="17">
+        <v>152.04999999999995</v>
+      </c>
+      <c r="L21" s="17">
+        <v>2151.1480000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="17">
+        <v>103.43</v>
+      </c>
+      <c r="C22" s="17">
+        <v>120.44500000000001</v>
+      </c>
+      <c r="D22" s="17">
+        <v>409.55500000000001</v>
+      </c>
+      <c r="E22" s="17">
+        <v>178.89100000000002</v>
+      </c>
+      <c r="F22" s="17">
+        <v>116.2</v>
+      </c>
+      <c r="G22" s="17">
+        <v>228.75600000000003</v>
+      </c>
+      <c r="H22" s="17">
+        <v>150.25200000000001</v>
+      </c>
+      <c r="I22" s="17">
+        <v>131.77800000000002</v>
+      </c>
+      <c r="J22" s="17">
+        <v>300.93700000000007</v>
+      </c>
+      <c r="K22" s="17">
+        <v>130.52199999999999</v>
+      </c>
+      <c r="L22" s="17">
+        <v>1870.7660000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="17">
+        <v>111.006</v>
+      </c>
+      <c r="C23" s="17">
+        <v>136.43800000000002</v>
+      </c>
+      <c r="D23" s="17">
+        <v>456.90600000000001</v>
+      </c>
+      <c r="E23" s="17">
+        <v>201.34900000000002</v>
+      </c>
+      <c r="F23" s="17">
+        <v>130.827</v>
+      </c>
+      <c r="G23" s="17">
+        <v>251.40600000000001</v>
+      </c>
+      <c r="H23" s="17">
+        <v>155.68400000000003</v>
+      </c>
+      <c r="I23" s="17">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="J23" s="17">
+        <v>319.82500000000005</v>
+      </c>
+      <c r="K23" s="17">
+        <v>141.303</v>
+      </c>
+      <c r="L23" s="17">
+        <v>2043.8540000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="17">
+        <v>112.99000000000002</v>
+      </c>
+      <c r="C24" s="17">
+        <v>133.142</v>
+      </c>
+      <c r="D24" s="17">
+        <v>432.70800000000003</v>
+      </c>
+      <c r="E24" s="17">
+        <v>188.85600000000002</v>
+      </c>
+      <c r="F24" s="17">
+        <v>129.11399999999998</v>
+      </c>
+      <c r="G24" s="17">
+        <v>245.78100000000006</v>
+      </c>
+      <c r="H24" s="17">
+        <v>156.32499999999999</v>
+      </c>
+      <c r="I24" s="17">
+        <v>141.29899999999998</v>
+      </c>
+      <c r="J24" s="17">
+        <v>313.95600000000007</v>
+      </c>
+      <c r="K24" s="17">
+        <v>137.828</v>
+      </c>
+      <c r="L24" s="17">
+        <v>1991.999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="17">
+        <v>98.518000000000015</v>
+      </c>
+      <c r="C25" s="17">
+        <v>114.45700000000002</v>
+      </c>
+      <c r="D25" s="17">
+        <v>411.76100000000002</v>
+      </c>
+      <c r="E25" s="17">
+        <v>157.23799999999997</v>
+      </c>
+      <c r="F25" s="17">
+        <v>105.85400000000001</v>
+      </c>
+      <c r="G25" s="17">
+        <v>199.86899999999997</v>
+      </c>
+      <c r="H25" s="17">
+        <v>137.363</v>
+      </c>
+      <c r="I25" s="17">
+        <v>124.30600000000001</v>
+      </c>
+      <c r="J25" s="17">
+        <v>257.80099999999999</v>
+      </c>
+      <c r="K25" s="17">
+        <v>124.499</v>
+      </c>
+      <c r="L25" s="17">
+        <v>1731.6660000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="17">
+        <v>111.697</v>
+      </c>
+      <c r="C26" s="17">
+        <v>120.01899999999999</v>
+      </c>
+      <c r="D26" s="17">
+        <v>425.90500000000009</v>
+      </c>
+      <c r="E26" s="17">
+        <v>157.94399999999999</v>
+      </c>
+      <c r="F26" s="17">
+        <v>110.45</v>
+      </c>
+      <c r="G26" s="17">
+        <v>202.65599999999998</v>
+      </c>
+      <c r="H26" s="17">
+        <v>153.88999999999999</v>
+      </c>
+      <c r="I26" s="17">
+        <v>133.56999999999996</v>
+      </c>
+      <c r="J26" s="17">
+        <v>279.60700000000003</v>
+      </c>
+      <c r="K26" s="17">
+        <v>135.64100000000002</v>
+      </c>
+      <c r="L26" s="17">
+        <v>1831.3790000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="17">
+        <v>91.993999999999986</v>
+      </c>
+      <c r="C27" s="17">
+        <v>90.7</v>
+      </c>
+      <c r="D27" s="17">
+        <v>356.572</v>
+      </c>
+      <c r="E27" s="17">
+        <v>118.15700000000002</v>
+      </c>
+      <c r="F27" s="17">
+        <v>79.431999999999988</v>
+      </c>
+      <c r="G27" s="17">
+        <v>139.21600000000001</v>
+      </c>
+      <c r="H27" s="17">
+        <v>134.75900000000001</v>
+      </c>
+      <c r="I27" s="17">
+        <v>105.11500000000001</v>
+      </c>
+      <c r="J27" s="17">
+        <v>196.13999999999996</v>
+      </c>
+      <c r="K27" s="17">
+        <v>122.11399999999999</v>
+      </c>
+      <c r="L27" s="17">
+        <v>1434.1990000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="17">
+        <v>80.479999999999961</v>
+      </c>
+      <c r="C28" s="17">
+        <v>76.384999999999991</v>
+      </c>
+      <c r="D28" s="17">
+        <v>263.3490000000001</v>
+      </c>
+      <c r="E28" s="17">
+        <v>98.891999999999982</v>
+      </c>
+      <c r="F28" s="17">
+        <v>61.866000000000014</v>
+      </c>
+      <c r="G28" s="17">
+        <v>115.74799999999998</v>
+      </c>
+      <c r="H28" s="17">
+        <v>114.46799999999999</v>
+      </c>
+      <c r="I28" s="17">
+        <v>90.445999999999984</v>
+      </c>
+      <c r="J28" s="17">
+        <v>146.62799999999999</v>
+      </c>
+      <c r="K28" s="17">
+        <v>103.73099999999999</v>
+      </c>
+      <c r="L28" s="17">
+        <v>1151.9929999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="17">
+        <v>43.441999999999993</v>
+      </c>
+      <c r="C29" s="17">
+        <v>44.253</v>
+      </c>
+      <c r="D29" s="17">
+        <v>155.75900000000001</v>
+      </c>
+      <c r="E29" s="17">
+        <v>61.987999999999985</v>
+      </c>
+      <c r="F29" s="17">
+        <v>33.684999999999995</v>
+      </c>
+      <c r="G29" s="17">
+        <v>66.321999999999989</v>
+      </c>
+      <c r="H29" s="17">
+        <v>69.669000000000011</v>
+      </c>
+      <c r="I29" s="17">
+        <v>57.185999999999986</v>
+      </c>
+      <c r="J29" s="17">
+        <v>75.953000000000003</v>
+      </c>
+      <c r="K29" s="17">
+        <v>60.731999999999985</v>
+      </c>
+      <c r="L29" s="17">
+        <v>668.98900000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="19">
+        <v>1168.316</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1260.1389999999999</v>
+      </c>
+      <c r="D30" s="19">
+        <v>4478.442</v>
+      </c>
+      <c r="E30" s="19">
+        <v>1717.6450000000002</v>
+      </c>
+      <c r="F30" s="19">
+        <v>1137.046</v>
+      </c>
+      <c r="G30" s="19">
+        <v>2060.0250000000001</v>
+      </c>
+      <c r="H30" s="19">
+        <v>1678.1820000000002</v>
+      </c>
+      <c r="I30" s="19">
+        <v>1407.0519999999999</v>
+      </c>
+      <c r="J30" s="19">
+        <v>2827.2000000000003</v>
+      </c>
+      <c r="K30" s="19">
+        <v>1476.645</v>
+      </c>
+      <c r="L30" s="19">
+        <v>19210.692000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add switchs to enable additional options. Options can be changed in code.
</commit_message>
<xml_diff>
--- a/cap_data.xlsx
+++ b/cap_data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="40">
   <si>
     <t>Column Labels</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>30 homes</t>
+  </si>
+  <si>
+    <t>10 homes no trade</t>
   </si>
 </sst>
 </file>
@@ -4857,10 +4860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:W33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35:P67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7178,6 +7181,1564 @@
       <c r="Y33">
         <f t="shared" si="2"/>
         <v>4.7685563973013503</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J36" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" t="s">
+        <v>29</v>
+      </c>
+      <c r="L36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M36" t="s">
+        <v>29</v>
+      </c>
+      <c r="N36" t="s">
+        <v>30</v>
+      </c>
+      <c r="O36" t="s">
+        <v>33</v>
+      </c>
+      <c r="P36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f>(D37-B37)/D37</f>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f>E37-C37</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f>(M37-K37)/M37</f>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f>N37-L37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>0.943660098333854</v>
+      </c>
+      <c r="C38">
+        <v>-6.48373870495322</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>-2.7901391590614599</v>
+      </c>
+      <c r="F38">
+        <f>(D38-B38)/D38</f>
+        <v>5.6339901666145997E-2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G67" si="6">E38-C38</f>
+        <v>3.6935995458917601</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>0.943660098333854</v>
+      </c>
+      <c r="L38">
+        <v>-6.48373870495322</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>-2.7901391590614599</v>
+      </c>
+      <c r="O38">
+        <f>(M38-K38)/M38</f>
+        <v>5.6339901666145997E-2</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ref="P38:P67" si="7">N38-L38</f>
+        <v>3.6935995458917601</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>0.975930079760575</v>
+      </c>
+      <c r="C39">
+        <v>-2.95459714350027</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>-0.89418382208228397</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39:F67" si="8">(D39-B39)/D39</f>
+        <v>2.4069920239425002E-2</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="6"/>
+        <v>2.0604133214179861</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>0.975930079760575</v>
+      </c>
+      <c r="L39">
+        <v>-2.95459714350027</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>-0.89418382208228397</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ref="O39:O67" si="9">(M39-K39)/M39</f>
+        <v>2.4069920239425002E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="7"/>
+        <v>2.0604133214179861</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>0.97650849555949704</v>
+      </c>
+      <c r="C40">
+        <v>-2.89332645041396</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>-0.18755178128633099</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="8"/>
+        <v>2.3491504440502964E-2</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="6"/>
+        <v>2.7057746691276288</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>0.97650849555949704</v>
+      </c>
+      <c r="L40">
+        <v>-2.89332645041396</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>-0.18755178128633099</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="9"/>
+        <v>2.3491504440502964E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="7"/>
+        <v>2.7057746691276288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.94033581934519905</v>
+      </c>
+      <c r="C41">
+        <v>-6.6074092154464497</v>
+      </c>
+      <c r="D41">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="E41">
+        <v>-2.2870179318339401E-2</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="8"/>
+        <v>5.966418065480001E-2</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="6"/>
+        <v>6.5845390361281106</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>0.94033581934519905</v>
+      </c>
+      <c r="L41">
+        <v>-6.6074092154464497</v>
+      </c>
+      <c r="M41">
+        <v>0.999999999999999</v>
+      </c>
+      <c r="N41">
+        <v>-2.2870179318339401E-2</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="9"/>
+        <v>5.966418065480001E-2</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="7"/>
+        <v>6.5845390361281106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>0.96499055784735899</v>
+      </c>
+      <c r="C42">
+        <v>-3.9904892782951999</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>-2.6029173217480599</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="8"/>
+        <v>3.5009442152641013E-2</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="6"/>
+        <v>1.3875719565471401</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="K42">
+        <v>0.96499055784735899</v>
+      </c>
+      <c r="L42">
+        <v>-3.9904892782951999</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>-2.6029173217480599</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="9"/>
+        <v>3.5009442152641013E-2</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="7"/>
+        <v>1.3875719565471401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>0.885361542706122</v>
+      </c>
+      <c r="C43">
+        <v>-11.848581267648701</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>-7.0412928426382999</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="8"/>
+        <v>0.114638457293878</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="6"/>
+        <v>4.8072884250104009</v>
+      </c>
+      <c r="J43">
+        <v>7</v>
+      </c>
+      <c r="K43">
+        <v>0.885361542706122</v>
+      </c>
+      <c r="L43">
+        <v>-11.848581267648701</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>-7.0412928426382999</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="9"/>
+        <v>0.114638457293878</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="7"/>
+        <v>4.8072884250104009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>0.92919614524405203</v>
+      </c>
+      <c r="C44">
+        <v>-6.8716690581105704</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>-6.2834623818526197E-2</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="8"/>
+        <v>7.080385475594797E-2</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="6"/>
+        <v>6.8088344342920442</v>
+      </c>
+      <c r="J44">
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <v>0.92919614524405203</v>
+      </c>
+      <c r="L44">
+        <v>-6.8716690581105704</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>-6.2834623818526197E-2</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="9"/>
+        <v>7.080385475594797E-2</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="7"/>
+        <v>6.8088344342920442</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>0.85759443810829505</v>
+      </c>
+      <c r="C45">
+        <v>-15.5098017726142</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>-5.2840787270748102</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="8"/>
+        <v>0.14240556189170495</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="6"/>
+        <v>10.225723045539389</v>
+      </c>
+      <c r="J45">
+        <v>9</v>
+      </c>
+      <c r="K45">
+        <v>0.85759443810829505</v>
+      </c>
+      <c r="L45">
+        <v>-15.5098017726142</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>-5.2840787270748102</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="9"/>
+        <v>0.14240556189170495</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="7"/>
+        <v>10.225723045539389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>0.94577008338239799</v>
+      </c>
+      <c r="C46">
+        <v>-6.4478422528058896</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>-2.43569040943308</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="8"/>
+        <v>5.4229916617602014E-2</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="6"/>
+        <v>4.0121518433728092</v>
+      </c>
+      <c r="J46">
+        <v>10</v>
+      </c>
+      <c r="K46">
+        <v>0.94577008338239799</v>
+      </c>
+      <c r="L46">
+        <v>-6.4478422528058896</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>-2.43569040943308</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="9"/>
+        <v>5.4229916617602014E-2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="7"/>
+        <v>4.0121518433728092</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>0.90634279010077701</v>
+      </c>
+      <c r="C47">
+        <v>-10.1601347804841</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>-5.1159675503696098</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="8"/>
+        <v>9.3657209899222993E-2</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="6"/>
+        <v>5.04416723011449</v>
+      </c>
+      <c r="J47">
+        <v>11</v>
+      </c>
+      <c r="K47">
+        <v>0.90634279010077701</v>
+      </c>
+      <c r="L47">
+        <v>-10.1601347804841</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>-5.1159675503696098</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="9"/>
+        <v>9.3657209899222993E-2</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="7"/>
+        <v>5.04416723011449</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>0.92626101872814803</v>
+      </c>
+      <c r="C48">
+        <v>-8.2398215444696401</v>
+      </c>
+      <c r="D48">
+        <v>0.92626101872814803</v>
+      </c>
+      <c r="E48">
+        <v>-8.2398215444696401</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>12</v>
+      </c>
+      <c r="K48">
+        <v>0.92626101872814803</v>
+      </c>
+      <c r="L48">
+        <v>-8.2398215444696401</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>-4.5647800728336696</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="9"/>
+        <v>7.3738981271851967E-2</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="7"/>
+        <v>3.6750414716359705</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>0.93882383657816304</v>
+      </c>
+      <c r="C49">
+        <v>-6.9808744322049403</v>
+      </c>
+      <c r="D49">
+        <v>0.93882383657816304</v>
+      </c>
+      <c r="E49">
+        <v>-6.9808744322049403</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>13</v>
+      </c>
+      <c r="K49">
+        <v>0.93882383657816304</v>
+      </c>
+      <c r="L49">
+        <v>-6.9808744322049403</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>-2.01903207463603</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="9"/>
+        <v>6.117616342183696E-2</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="7"/>
+        <v>4.9618423575689103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>0.92356093636730296</v>
+      </c>
+      <c r="C50">
+        <v>-8.5093520086487793</v>
+      </c>
+      <c r="D50">
+        <v>0.92356093636730296</v>
+      </c>
+      <c r="E50">
+        <v>-8.5093520086487793</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>14</v>
+      </c>
+      <c r="K50">
+        <v>0.92356093636730296</v>
+      </c>
+      <c r="L50">
+        <v>-8.5093520086487793</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>-6.3304759449954497</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="9"/>
+        <v>7.6439063632697035E-2</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="7"/>
+        <v>2.1788760636533295</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>0.96435234406574699</v>
+      </c>
+      <c r="C51">
+        <v>-4.1211802104494604</v>
+      </c>
+      <c r="D51">
+        <v>0.96435234406574699</v>
+      </c>
+      <c r="E51">
+        <v>-4.1211802104494604</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>15</v>
+      </c>
+      <c r="K51">
+        <v>0.96435234406574699</v>
+      </c>
+      <c r="L51">
+        <v>-4.1211802104494604</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>-1.08357121731953</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="9"/>
+        <v>3.5647655934253009E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="7"/>
+        <v>3.0376089931299304</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>0.91779986823675097</v>
+      </c>
+      <c r="C52">
+        <v>-8.6779606699124496</v>
+      </c>
+      <c r="D52">
+        <v>0.91779986823675097</v>
+      </c>
+      <c r="E52">
+        <v>-8.6779606699124496</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+      <c r="K52">
+        <v>0.91779986823675097</v>
+      </c>
+      <c r="L52">
+        <v>-8.6779606699124496</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>-6.2169954709728401</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="9"/>
+        <v>8.2200131763249029E-2</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="7"/>
+        <v>2.4609651989396095</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>17</v>
+      </c>
+      <c r="B53">
+        <v>0.95737164318198098</v>
+      </c>
+      <c r="C53">
+        <v>-4.9227659903648897</v>
+      </c>
+      <c r="D53">
+        <v>0.95737164318198098</v>
+      </c>
+      <c r="E53">
+        <v>-4.9227659903648897</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>17</v>
+      </c>
+      <c r="K53">
+        <v>0.95737164318198098</v>
+      </c>
+      <c r="L53">
+        <v>-4.9227659903648897</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>-2.7144946216607502</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="9"/>
+        <v>4.262835681801902E-2</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="7"/>
+        <v>2.2082713687041395</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>18</v>
+      </c>
+      <c r="B54">
+        <v>0.88521679355444105</v>
+      </c>
+      <c r="C54">
+        <v>-10.5869716410379</v>
+      </c>
+      <c r="D54">
+        <v>0.88521679355444105</v>
+      </c>
+      <c r="E54">
+        <v>-10.5869716410379</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>18</v>
+      </c>
+      <c r="K54">
+        <v>0.88521679355444105</v>
+      </c>
+      <c r="L54">
+        <v>-10.5869716410379</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>-6.1972864279504201</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="9"/>
+        <v>0.11478320644555895</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="7"/>
+        <v>4.3896852130874802</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>19</v>
+      </c>
+      <c r="B55">
+        <v>0.93236349091189996</v>
+      </c>
+      <c r="C55">
+        <v>-8.3127261746205701</v>
+      </c>
+      <c r="D55">
+        <v>0.93236349091189996</v>
+      </c>
+      <c r="E55">
+        <v>-8.3127261746205701</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>19</v>
+      </c>
+      <c r="K55">
+        <v>0.93236349091189996</v>
+      </c>
+      <c r="L55">
+        <v>-8.3127261746205701</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>-2.2996954397043901</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="9"/>
+        <v>6.7636509088100039E-2</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="7"/>
+        <v>6.01303073491618</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56">
+        <v>0.87871975632937604</v>
+      </c>
+      <c r="C56">
+        <v>-12.955951433283801</v>
+      </c>
+      <c r="D56">
+        <v>0.87871975632937604</v>
+      </c>
+      <c r="E56">
+        <v>-12.955951433283801</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>20</v>
+      </c>
+      <c r="K56">
+        <v>0.87871975632937604</v>
+      </c>
+      <c r="L56">
+        <v>-12.955951433283801</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <v>-5.6149316000307703</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="9"/>
+        <v>0.12128024367062396</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="7"/>
+        <v>7.3410198332530303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>21</v>
+      </c>
+      <c r="B57">
+        <v>0.92660817773548398</v>
+      </c>
+      <c r="C57">
+        <v>-8.2168141162233699</v>
+      </c>
+      <c r="D57">
+        <v>0.92660817773548398</v>
+      </c>
+      <c r="E57">
+        <v>-8.2168141162233699</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>21</v>
+      </c>
+      <c r="K57">
+        <v>0.92660817773548398</v>
+      </c>
+      <c r="L57">
+        <v>-8.2168141162233699</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1.9803813406169299</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="9"/>
+        <v>7.3391822264516016E-2</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="7"/>
+        <v>10.1971954568403</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>22</v>
+      </c>
+      <c r="B58">
+        <v>0.83317954717155396</v>
+      </c>
+      <c r="C58">
+        <v>-16.488872365874801</v>
+      </c>
+      <c r="D58">
+        <v>0.83317954717155396</v>
+      </c>
+      <c r="E58">
+        <v>-16.488872365874801</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>22</v>
+      </c>
+      <c r="K58">
+        <v>0.83317954717155396</v>
+      </c>
+      <c r="L58">
+        <v>-16.488872365874801</v>
+      </c>
+      <c r="M58">
+        <v>0.83317954717155396</v>
+      </c>
+      <c r="N58">
+        <v>-16.488872365874801</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>23</v>
+      </c>
+      <c r="B59">
+        <v>0.95633087832760799</v>
+      </c>
+      <c r="C59">
+        <v>-5.1448653016470596</v>
+      </c>
+      <c r="D59">
+        <v>0.95633087832760799</v>
+      </c>
+      <c r="E59">
+        <v>-5.1448653016470596</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>23</v>
+      </c>
+      <c r="K59">
+        <v>0.95633087832760799</v>
+      </c>
+      <c r="L59">
+        <v>-5.1448653016470596</v>
+      </c>
+      <c r="M59">
+        <v>0.95633087832760799</v>
+      </c>
+      <c r="N59">
+        <v>-5.1448653016470596</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>24</v>
+      </c>
+      <c r="B60">
+        <v>0.93954279815962505</v>
+      </c>
+      <c r="C60">
+        <v>-6.91239962335748</v>
+      </c>
+      <c r="D60">
+        <v>0.93954279815962505</v>
+      </c>
+      <c r="E60">
+        <v>-6.91239962335748</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>24</v>
+      </c>
+      <c r="K60">
+        <v>0.93954279815962505</v>
+      </c>
+      <c r="L60">
+        <v>-6.91239962335748</v>
+      </c>
+      <c r="M60">
+        <v>0.93954279815962505</v>
+      </c>
+      <c r="N60">
+        <v>-6.91239962335748</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>25</v>
+      </c>
+      <c r="B61">
+        <v>0.953916461886269</v>
+      </c>
+      <c r="C61">
+        <v>-5.2244455259564999</v>
+      </c>
+      <c r="D61">
+        <v>0.953916461886269</v>
+      </c>
+      <c r="E61">
+        <v>-5.2244455259564999</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>25</v>
+      </c>
+      <c r="K61">
+        <v>0.953916461886269</v>
+      </c>
+      <c r="L61">
+        <v>-5.2244455259564999</v>
+      </c>
+      <c r="M61">
+        <v>0.953916461886269</v>
+      </c>
+      <c r="N61">
+        <v>-5.2244455259564999</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>26</v>
+      </c>
+      <c r="B62">
+        <v>0.95445205885390105</v>
+      </c>
+      <c r="C62">
+        <v>-5.0938925498123204</v>
+      </c>
+      <c r="D62">
+        <v>0.95445205885390105</v>
+      </c>
+      <c r="E62">
+        <v>-5.0938925498123204</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>26</v>
+      </c>
+      <c r="K62">
+        <v>0.95445205885390105</v>
+      </c>
+      <c r="L62">
+        <v>-5.0938925498123204</v>
+      </c>
+      <c r="M62">
+        <v>0.95445205885390105</v>
+      </c>
+      <c r="N62">
+        <v>-5.0938925498123204</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>27</v>
+      </c>
+      <c r="B63">
+        <v>0.886466289769268</v>
+      </c>
+      <c r="C63">
+        <v>-11.751200787598</v>
+      </c>
+      <c r="D63">
+        <v>0.886466289769268</v>
+      </c>
+      <c r="E63">
+        <v>-11.751200787598</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>27</v>
+      </c>
+      <c r="K63">
+        <v>0.886466289769268</v>
+      </c>
+      <c r="L63">
+        <v>-11.751200787598</v>
+      </c>
+      <c r="M63">
+        <v>0.886466289769268</v>
+      </c>
+      <c r="N63">
+        <v>-11.751200787598</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>28</v>
+      </c>
+      <c r="B64">
+        <v>0.79148014536841305</v>
+      </c>
+      <c r="C64">
+        <v>-17.652432495623</v>
+      </c>
+      <c r="D64">
+        <v>0.79148014536841305</v>
+      </c>
+      <c r="E64">
+        <v>-17.652432495623</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>28</v>
+      </c>
+      <c r="K64">
+        <v>0.79148014536841305</v>
+      </c>
+      <c r="L64">
+        <v>-17.652432495623</v>
+      </c>
+      <c r="M64">
+        <v>0.79148014536841305</v>
+      </c>
+      <c r="N64">
+        <v>-17.652432495623</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>29</v>
+      </c>
+      <c r="B65">
+        <v>0.88469386653775095</v>
+      </c>
+      <c r="C65">
+        <v>-13.0536402344504</v>
+      </c>
+      <c r="D65">
+        <v>0.88469386653775095</v>
+      </c>
+      <c r="E65">
+        <v>-13.0536402344504</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>29</v>
+      </c>
+      <c r="K65">
+        <v>0.88469386653775095</v>
+      </c>
+      <c r="L65">
+        <v>-13.0536402344504</v>
+      </c>
+      <c r="M65">
+        <v>0.88469386653775095</v>
+      </c>
+      <c r="N65">
+        <v>-13.0536402344504</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>30</v>
+      </c>
+      <c r="B66">
+        <v>0.92092973468673001</v>
+      </c>
+      <c r="C66">
+        <v>-8.99554061248773</v>
+      </c>
+      <c r="D66">
+        <v>0.92092973468673001</v>
+      </c>
+      <c r="E66">
+        <v>-8.99554061248773</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>30</v>
+      </c>
+      <c r="K66">
+        <v>0.92092973468673001</v>
+      </c>
+      <c r="L66">
+        <v>-8.99554061248773</v>
+      </c>
+      <c r="M66">
+        <v>0.92092973468673001</v>
+      </c>
+      <c r="N66">
+        <v>-8.99554061248773</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>31</v>
+      </c>
+      <c r="B67">
+        <v>0.951551272462275</v>
+      </c>
+      <c r="C67">
+        <v>-5.6698319544087301</v>
+      </c>
+      <c r="D67">
+        <v>0.951551272462275</v>
+      </c>
+      <c r="E67">
+        <v>-5.6698319544087301</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>31</v>
+      </c>
+      <c r="K67">
+        <v>0.951551272462275</v>
+      </c>
+      <c r="L67">
+        <v>-5.6698319544087301</v>
+      </c>
+      <c r="M67">
+        <v>0.951551272462275</v>
+      </c>
+      <c r="N67">
+        <v>-5.6698319544087301</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>